<commit_message>
Added 2x6 board prices
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2BA7545D-E564-4242-B561-CF7E59CE6862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ECB15B36-CBF9-4345-A502-0508311F015C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="-21100" windowWidth="29720" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
+    <workbookView xWindow="3580" yWindow="-21100" windowWidth="29720" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_2" sheetId="1" r:id="rId1"/>
@@ -1082,9 +1082,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1461,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0679CAE-7790-0146-A436-E7EEAE9C9294}">
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O119" sqref="O119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1502,13 +1502,13 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="L1" t="s">
@@ -1544,7 +1544,7 @@
         <f>INT(E2/12) &amp; " ft " &amp; MOD(E2,12) &amp; " in"</f>
         <v>8 ft 0 in</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J2">
@@ -1574,7 +1574,7 @@
         <f>INT(E3/12) &amp; " ft " &amp; MOD(E3,12) &amp; " in"</f>
         <v>4 ft 0 in</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J3">
@@ -1607,19 +1607,20 @@
         <f>INT(E4/12) &amp; " ft " &amp; MOD(E4,12) &amp; " in"</f>
         <v>6 ft 6 in</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J4">
         <v>17</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
         <v>120</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>6</v>
       </c>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1647,19 +1648,20 @@
         <f>INT(E5/12) &amp; " ft " &amp; MOD(E5,12) &amp; " in"</f>
         <v>6 ft 5.75 in</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J5">
         <v>18</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
         <v>144</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>1</v>
       </c>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1687,19 +1689,20 @@
         <f>INT(E6/12) &amp; " ft " &amp; MOD(E6,12) &amp; " in"</f>
         <v>9 ft 3 in</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J6">
         <v>19</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
         <v>168</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="2">
         <v>12</v>
       </c>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1727,19 +1730,20 @@
         <f>INT(E7/12) &amp; " ft " &amp; MOD(E7,12) &amp; " in"</f>
         <v>9 ft 3 in</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J7">
         <v>20</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
         <v>240</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="2">
         <v>1</v>
       </c>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1767,13 +1771,16 @@
         <f>INT(E8/12) &amp; " ft " &amp; MOD(E8,12) &amp; " in"</f>
         <v>13 ft 3 in</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J8">
         <v>21</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1801,13 +1808,16 @@
         <f>INT(E9/12) &amp; " ft " &amp; MOD(E9,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J9">
         <v>22</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1835,13 +1845,16 @@
         <f>INT(E10/12) &amp; " ft " &amp; MOD(E10,12) &amp; " in"</f>
         <v>4 ft 4.75 in</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J10">
         <v>23</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1869,13 +1882,16 @@
         <f>INT(E11/12) &amp; " ft " &amp; MOD(E11,12) &amp; " in"</f>
         <v>6 ft 6 in</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J11">
         <v>29</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1900,14 +1916,16 @@
         <f>INT(E12/12) &amp; " ft " &amp; MOD(E12,12) &amp; " in"</f>
         <v>2 ft 6 in</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J12">
         <v>30</v>
       </c>
-      <c r="K12" s="3"/>
-      <c r="N12">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2">
         <v>327.10000000000002</v>
       </c>
     </row>
@@ -1937,7 +1955,7 @@
         <f>INT(E13/12) &amp; " ft " &amp; MOD(E13,12) &amp; " in"</f>
         <v>16 ft 0 in</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J13">
@@ -1970,7 +1988,7 @@
         <f>INT(E14/12) &amp; " ft " &amp; MOD(E14,12) &amp; " in"</f>
         <v>12 ft 8 in</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J14">
@@ -2003,7 +2021,7 @@
         <f>INT(E15/12) &amp; " ft " &amp; MOD(E15,12) &amp; " in"</f>
         <v>6 ft 10 in</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J15">
@@ -2033,15 +2051,18 @@
         <f>INT(E16/12) &amp; " ft " &amp; MOD(E16,12) &amp; " in"</f>
         <v>8 ft 0 in</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>162</v>
       </c>
@@ -2064,15 +2085,18 @@
         <f>INT(E17/12) &amp; " ft " &amp; MOD(E17,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J17">
         <v>2</v>
       </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -2095,16 +2119,18 @@
         <f>INT(E18/12) &amp; " ft " &amp; MOD(E18,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J18">
         <v>3</v>
       </c>
-      <c r="K18" s="3"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>165</v>
       </c>
@@ -2127,16 +2153,18 @@
         <f>INT(E19/12) &amp; " ft " &amp; MOD(E19,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J19">
         <v>4</v>
       </c>
-      <c r="K19" s="3"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -2159,16 +2187,18 @@
         <f>INT(E20/12) &amp; " ft " &amp; MOD(E20,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J20">
         <v>5</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -2191,16 +2221,18 @@
         <f>INT(E21/12) &amp; " ft " &amp; MOD(E21,12) &amp; " in"</f>
         <v>14 ft 0 in</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J21">
         <v>6</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -2223,16 +2255,18 @@
         <f>INT(E22/12) &amp; " ft " &amp; MOD(E22,12) &amp; " in"</f>
         <v>14 ft 0 in</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J22">
         <v>7</v>
       </c>
-      <c r="K22" s="3"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>170</v>
       </c>
@@ -2255,16 +2289,18 @@
         <f>INT(E23/12) &amp; " ft " &amp; MOD(E23,12) &amp; " in"</f>
         <v>16 ft 0 in</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J23">
         <v>8</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>171</v>
       </c>
@@ -2287,16 +2323,18 @@
         <f>INT(E24/12) &amp; " ft " &amp; MOD(E24,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J24">
         <v>9</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>176</v>
       </c>
@@ -2319,16 +2357,18 @@
         <f>INT(E25/12) &amp; " ft " &amp; MOD(E25,12) &amp; " in"</f>
         <v>11 ft 8.5 in</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J25">
         <v>10</v>
       </c>
-      <c r="K25" s="3"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>175</v>
       </c>
@@ -2351,15 +2391,18 @@
         <f>INT(E26/12) &amp; " ft " &amp; MOD(E26,12) &amp; " in"</f>
         <v>1 ft 10.13 in</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J26">
         <v>11</v>
       </c>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>174</v>
       </c>
@@ -2382,15 +2425,18 @@
         <f>INT(E27/12) &amp; " ft " &amp; MOD(E27,12) &amp; " in"</f>
         <v>1 ft 9.25 in</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J27">
         <v>12</v>
       </c>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -2416,15 +2462,20 @@
         <f>INT(E28/12) &amp; " ft " &amp; MOD(E28,12) &amp; " in"</f>
         <v>6 ft 3.38 in</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J28">
         <v>84</v>
       </c>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2447,14 +2498,14 @@
         <f>INT(E29/12) &amp; " ft " &amp; MOD(E29,12) &amp; " in"</f>
         <v>3 ft 9 in</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J29">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2477,14 +2528,14 @@
         <f>INT(E30/12) &amp; " ft " &amp; MOD(E30,12) &amp; " in"</f>
         <v>8 ft 7 in</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J30">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2507,14 +2558,14 @@
         <f>INT(E31/12) &amp; " ft " &amp; MOD(E31,12) &amp; " in"</f>
         <v>5 ft 6 in</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J31">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2540,7 +2591,7 @@
         <f>INT(E32/12) &amp; " ft " &amp; MOD(E32,12) &amp; " in"</f>
         <v>8 ft 7 in</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J32">
@@ -2570,7 +2621,7 @@
         <f>INT(E33/12) &amp; " ft " &amp; MOD(E33,12) &amp; " in"</f>
         <v>2 ft 0.5 in</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J33">
@@ -2603,7 +2654,7 @@
         <f>INT(E34/12) &amp; " ft " &amp; MOD(E34,12) &amp; " in"</f>
         <v>11 ft 4 in</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J34">
@@ -2633,7 +2684,7 @@
         <f>INT(E35/12) &amp; " ft " &amp; MOD(E35,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="I35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J35">
@@ -2663,7 +2714,7 @@
         <f>INT(E36/12) &amp; " ft " &amp; MOD(E36,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J36">
@@ -2696,7 +2747,7 @@
         <f>INT(E37/12) &amp; " ft " &amp; MOD(E37,12) &amp; " in"</f>
         <v>10 ft 5.75 in</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="I37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J37">
@@ -2729,7 +2780,7 @@
         <f>INT(E38/12) &amp; " ft " &amp; MOD(E38,12) &amp; " in"</f>
         <v>16 ft 0 in</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I38" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J38">
@@ -2762,7 +2813,7 @@
         <f>INT(E39/12) &amp; " ft " &amp; MOD(E39,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J39">
@@ -2795,7 +2846,7 @@
         <f>INT(E40/12) &amp; " ft " &amp; MOD(E40,12) &amp; " in"</f>
         <v>6 ft 11 in</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J40">
@@ -2825,7 +2876,7 @@
         <f>INT(E41/12) &amp; " ft " &amp; MOD(E41,12) &amp; " in"</f>
         <v>1 ft 0 in</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J41">
@@ -2855,7 +2906,7 @@
         <f>INT(E42/12) &amp; " ft " &amp; MOD(E42,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="I42" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J42">
@@ -2885,7 +2936,7 @@
         <f>INT(E43/12) &amp; " ft " &amp; MOD(E43,12) &amp; " in"</f>
         <v>4 ft 2 in</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="I43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J43">
@@ -2915,7 +2966,7 @@
         <f>INT(E44/12) &amp; " ft " &amp; MOD(E44,12) &amp; " in"</f>
         <v>4 ft 0 in</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="I44" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J44">
@@ -2945,7 +2996,7 @@
         <f>INT(E45/12) &amp; " ft " &amp; MOD(E45,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="I45" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J45">
@@ -2978,7 +3029,7 @@
         <f>INT(E46/12) &amp; " ft " &amp; MOD(E46,12) &amp; " in"</f>
         <v>14 ft 0 in</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J46">
@@ -3011,7 +3062,7 @@
         <f>INT(E47/12) &amp; " ft " &amp; MOD(E47,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J47">
@@ -3041,7 +3092,7 @@
         <f>INT(E48/12) &amp; " ft " &amp; MOD(E48,12) &amp; " in"</f>
         <v>4 ft 2 in</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J48">
@@ -3074,7 +3125,7 @@
         <f>INT(E49/12) &amp; " ft " &amp; MOD(E49,12) &amp; " in"</f>
         <v>7 ft 6 in</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J49">
@@ -3107,7 +3158,7 @@
         <f>INT(E50/12) &amp; " ft " &amp; MOD(E50,12) &amp; " in"</f>
         <v>6 ft 10 in</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="I50" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J50">
@@ -3140,7 +3191,7 @@
         <f>INT(E51/12) &amp; " ft " &amp; MOD(E51,12) &amp; " in"</f>
         <v>6 ft 3.38 in</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="I51" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J51">
@@ -3173,7 +3224,7 @@
         <f>INT(E52/12) &amp; " ft " &amp; MOD(E52,12) &amp; " in"</f>
         <v>12 ft 3 in</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="I52" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J52">
@@ -3203,7 +3254,7 @@
         <f>INT(E53/12) &amp; " ft " &amp; MOD(E53,12) &amp; " in"</f>
         <v>4 ft 0 in</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="I53" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J53">
@@ -3233,7 +3284,7 @@
         <f>INT(E54/12) &amp; " ft " &amp; MOD(E54,12) &amp; " in"</f>
         <v>6 ft 8 in</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J54">
@@ -3266,7 +3317,7 @@
         <f>INT(E55/12) &amp; " ft " &amp; MOD(E55,12) &amp; " in"</f>
         <v>3 ft 2.5 in</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="I55" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J55">
@@ -3296,7 +3347,7 @@
         <f>INT(E56/12) &amp; " ft " &amp; MOD(E56,12) &amp; " in"</f>
         <v>6 ft 9 in</v>
       </c>
-      <c r="I56" s="2" t="s">
+      <c r="I56" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J56">
@@ -3329,7 +3380,7 @@
         <f>INT(E57/12) &amp; " ft " &amp; MOD(E57,12) &amp; " in"</f>
         <v>16 ft 0 in</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="I57" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J57">
@@ -3362,7 +3413,7 @@
         <f>INT(E58/12) &amp; " ft " &amp; MOD(E58,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="I58" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J58">
@@ -3392,7 +3443,7 @@
         <f>INT(E59/12) &amp; " ft " &amp; MOD(E59,12) &amp; " in"</f>
         <v>3 ft 10 in</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="I59" s="1" t="s">
         <v>119</v>
       </c>
       <c r="J59">
@@ -3425,7 +3476,7 @@
         <f>INT(E60/12) &amp; " ft " &amp; MOD(E60,12) &amp; " in"</f>
         <v>7 ft 4 in</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="I60" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J60">
@@ -3458,7 +3509,7 @@
         <f>INT(E61/12) &amp; " ft " &amp; MOD(E61,12) &amp; " in"</f>
         <v>7 ft 6 in</v>
       </c>
-      <c r="I61" s="2" t="s">
+      <c r="I61" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J61">
@@ -3491,7 +3542,7 @@
         <f>INT(E62/12) &amp; " ft " &amp; MOD(E62,12) &amp; " in"</f>
         <v>3 ft 8.5 in</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="I62" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J62">
@@ -3524,7 +3575,7 @@
         <f>INT(E63/12) &amp; " ft " &amp; MOD(E63,12) &amp; " in"</f>
         <v>6 ft 9 in</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="I63" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J63">
@@ -3554,7 +3605,7 @@
         <f>INT(E64/12) &amp; " ft " &amp; MOD(E64,12) &amp; " in"</f>
         <v>3 ft 8.5 in</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="I64" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J64">
@@ -3584,7 +3635,7 @@
         <f>INT(E65/12) &amp; " ft " &amp; MOD(E65,12) &amp; " in"</f>
         <v>2 ft 0.5 in</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I65" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J65">
@@ -3614,7 +3665,7 @@
         <f>INT(E66/12) &amp; " ft " &amp; MOD(E66,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="I66" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J66">
@@ -3644,7 +3695,7 @@
         <f>INT(E67/12) &amp; " ft " &amp; MOD(E67,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="I67" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J67">
@@ -3674,7 +3725,7 @@
         <f>INT(E68/12) &amp; " ft " &amp; MOD(E68,12) &amp; " in"</f>
         <v>14 ft 0 in</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I68" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J68">
@@ -3704,7 +3755,7 @@
         <f>INT(E69/12) &amp; " ft " &amp; MOD(E69,12) &amp; " in"</f>
         <v>4 ft 0 in</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="I69" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J69">
@@ -3734,7 +3785,7 @@
         <f>INT(E70/12) &amp; " ft " &amp; MOD(E70,12) &amp; " in"</f>
         <v>3 ft 0.5 in</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="I70" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J70">
@@ -3764,7 +3815,7 @@
         <f>INT(E71/12) &amp; " ft " &amp; MOD(E71,12) &amp; " in"</f>
         <v>1 ft 10.5 in</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I71" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J71">
@@ -3797,7 +3848,7 @@
         <f>INT(E72/12) &amp; " ft " &amp; MOD(E72,12) &amp; " in"</f>
         <v>6 ft 3.38 in</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I72" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J72">
@@ -3827,7 +3878,7 @@
         <f>INT(E73/12) &amp; " ft " &amp; MOD(E73,12) &amp; " in"</f>
         <v>3 ft 0.5 in</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="I73" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J73">
@@ -3857,7 +3908,7 @@
         <f>INT(E74/12) &amp; " ft " &amp; MOD(E74,12) &amp; " in"</f>
         <v>6 ft 8 in</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="I74" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J74">
@@ -3887,7 +3938,7 @@
         <f>INT(E75/12) &amp; " ft " &amp; MOD(E75,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I75" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J75">
@@ -3917,7 +3968,7 @@
         <f>INT(E76/12) &amp; " ft " &amp; MOD(E76,12) &amp; " in"</f>
         <v>4 ft 1 in</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I76" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J76">
@@ -3947,7 +3998,7 @@
         <f>INT(E77/12) &amp; " ft " &amp; MOD(E77,12) &amp; " in"</f>
         <v>1 ft 8 in</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I77" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J77">
@@ -3980,7 +4031,7 @@
         <f>INT(E78/12) &amp; " ft " &amp; MOD(E78,12) &amp; " in"</f>
         <v>8 ft 4 in</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I78" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J78">
@@ -4013,7 +4064,7 @@
         <f>INT(E79/12) &amp; " ft " &amp; MOD(E79,12) &amp; " in"</f>
         <v>8 ft 8 in</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I79" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J79">
@@ -4046,7 +4097,7 @@
         <f>INT(E80/12) &amp; " ft " &amp; MOD(E80,12) &amp; " in"</f>
         <v>9 ft 0 in</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I80" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J80">
@@ -4079,7 +4130,7 @@
         <f>INT(E81/12) &amp; " ft " &amp; MOD(E81,12) &amp; " in"</f>
         <v>9 ft 4 in</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I81" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J81">
@@ -4112,7 +4163,7 @@
         <f>INT(E82/12) &amp; " ft " &amp; MOD(E82,12) &amp; " in"</f>
         <v>9 ft 8 in</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I82" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J82">
@@ -4145,7 +4196,7 @@
         <f>INT(E83/12) &amp; " ft " &amp; MOD(E83,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I83" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J83">
@@ -4178,7 +4229,7 @@
         <f>INT(E84/12) &amp; " ft " &amp; MOD(E84,12) &amp; " in"</f>
         <v>7 ft 10 in</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I84" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J84">
@@ -4211,7 +4262,7 @@
         <f>INT(E85/12) &amp; " ft " &amp; MOD(E85,12) &amp; " in"</f>
         <v>8 ft 2 in</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I85" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J85">
@@ -4244,7 +4295,7 @@
         <f>INT(E86/12) &amp; " ft " &amp; MOD(E86,12) &amp; " in"</f>
         <v>8 ft 10 in</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I86" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J86">
@@ -4277,7 +4328,7 @@
         <f>INT(E87/12) &amp; " ft " &amp; MOD(E87,12) &amp; " in"</f>
         <v>8 ft 6 in</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I87" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J87">
@@ -4310,7 +4361,7 @@
         <f>INT(E88/12) &amp; " ft " &amp; MOD(E88,12) &amp; " in"</f>
         <v>2 ft 4.25 in</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="I88" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J88">
@@ -4343,7 +4394,7 @@
         <f>INT(E89/12) &amp; " ft " &amp; MOD(E89,12) &amp; " in"</f>
         <v>2 ft 0.25 in</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I89" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J89">
@@ -4376,7 +4427,7 @@
         <f>INT(E90/12) &amp; " ft " &amp; MOD(E90,12) &amp; " in"</f>
         <v>1 ft 8.25 in</v>
       </c>
-      <c r="I90" s="2" t="s">
+      <c r="I90" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J90">
@@ -4409,7 +4460,7 @@
         <f>INT(E91/12) &amp; " ft " &amp; MOD(E91,12) &amp; " in"</f>
         <v>1 ft 4.25 in</v>
       </c>
-      <c r="I91" s="2" t="s">
+      <c r="I91" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J91">
@@ -4442,7 +4493,7 @@
         <f>INT(E92/12) &amp; " ft " &amp; MOD(E92,12) &amp; " in"</f>
         <v>1 ft 0.25 in</v>
       </c>
-      <c r="I92" s="2" t="s">
+      <c r="I92" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J92">
@@ -4475,7 +4526,7 @@
         <f>INT(E93/12) &amp; " ft " &amp; MOD(E93,12) &amp; " in"</f>
         <v>0 ft 8.25 in</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I93" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J93">
@@ -4505,7 +4556,7 @@
         <f>INT(E94/12) &amp; " ft " &amp; MOD(E94,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I94" s="2" t="s">
+      <c r="I94" s="1" t="s">
         <v>161</v>
       </c>
       <c r="J94">
@@ -4535,7 +4586,7 @@
         <f>INT(E95/12) &amp; " ft " &amp; MOD(E95,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I95" s="2" t="s">
+      <c r="I95" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J95">
@@ -4568,7 +4619,7 @@
         <f>INT(E96/12) &amp; " ft " &amp; MOD(E96,12) &amp; " in"</f>
         <v>2 ft 3 in</v>
       </c>
-      <c r="I96" s="2" t="s">
+      <c r="I96" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J96">
@@ -4601,7 +4652,7 @@
         <f>INT(E97/12) &amp; " ft " &amp; MOD(E97,12) &amp; " in"</f>
         <v>2 ft 6 in</v>
       </c>
-      <c r="I97" s="2" t="s">
+      <c r="I97" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J97">
@@ -4631,7 +4682,7 @@
         <f>INT(E98/12) &amp; " ft " &amp; MOD(E98,12) &amp; " in"</f>
         <v>7 ft 4 in</v>
       </c>
-      <c r="I98" s="2" t="s">
+      <c r="I98" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J98">
@@ -4661,7 +4712,7 @@
         <f>INT(E99/12) &amp; " ft " &amp; MOD(E99,12) &amp; " in"</f>
         <v>4 ft 0 in</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="I99" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J99">
@@ -4691,7 +4742,7 @@
         <f>INT(E100/12) &amp; " ft " &amp; MOD(E100,12) &amp; " in"</f>
         <v>1 ft 0 in</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I100" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J100">
@@ -4724,7 +4775,7 @@
         <f>INT(E101/12) &amp; " ft " &amp; MOD(E101,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="I101" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J101">
@@ -4757,7 +4808,7 @@
         <f>INT(E102/12) &amp; " ft " &amp; MOD(E102,12) &amp; " in"</f>
         <v>8 ft 1 in</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="I102" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J102">
@@ -4790,7 +4841,7 @@
         <f>INT(E103/12) &amp; " ft " &amp; MOD(E103,12) &amp; " in"</f>
         <v>8 ft 5 in</v>
       </c>
-      <c r="I103" s="2" t="s">
+      <c r="I103" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J103">
@@ -4823,7 +4874,7 @@
         <f>INT(E104/12) &amp; " ft " &amp; MOD(E104,12) &amp; " in"</f>
         <v>9 ft 1 in</v>
       </c>
-      <c r="I104" s="2" t="s">
+      <c r="I104" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J104">
@@ -4856,7 +4907,7 @@
         <f>INT(E105/12) &amp; " ft " &amp; MOD(E105,12) &amp; " in"</f>
         <v>9 ft 4 in</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="I105" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J105">
@@ -4889,7 +4940,7 @@
         <f>INT(E106/12) &amp; " ft " &amp; MOD(E106,12) &amp; " in"</f>
         <v>7 ft 1 in</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="I106" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J106">
@@ -4922,7 +4973,7 @@
         <f>INT(E107/12) &amp; " ft " &amp; MOD(E107,12) &amp; " in"</f>
         <v>7 ft 5 in</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="I107" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J107">
@@ -4955,7 +5006,7 @@
         <f>INT(E108/12) &amp; " ft " &amp; MOD(E108,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="I108" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J108">
@@ -4988,7 +5039,7 @@
         <f>INT(E109/12) &amp; " ft " &amp; MOD(E109,12) &amp; " in"</f>
         <v>8 ft 1 in</v>
       </c>
-      <c r="I109" s="2" t="s">
+      <c r="I109" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J109">
@@ -5021,7 +5072,7 @@
         <f>INT(E110/12) &amp; " ft " &amp; MOD(E110,12) &amp; " in"</f>
         <v>1 ft 4 in</v>
       </c>
-      <c r="I110" s="2" t="s">
+      <c r="I110" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J110">
@@ -5054,7 +5105,7 @@
         <f>INT(E111/12) &amp; " ft " &amp; MOD(E111,12) &amp; " in"</f>
         <v>1 ft 7 in</v>
       </c>
-      <c r="I111" s="2" t="s">
+      <c r="I111" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J111">
@@ -5084,14 +5135,14 @@
         <f>INT(E112/12) &amp; " ft " &amp; MOD(E112,12) &amp; " in"</f>
         <v>1 ft 8 in</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="I112" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J112">
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>99</v>
       </c>
@@ -5117,14 +5168,14 @@
         <f>INT(E113/12) &amp; " ft " &amp; MOD(E113,12) &amp; " in"</f>
         <v>0 ft 6 in</v>
       </c>
-      <c r="I113" s="2" t="s">
+      <c r="I113" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J113">
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>101</v>
       </c>
@@ -5150,14 +5201,14 @@
         <f>INT(E114/12) &amp; " ft " &amp; MOD(E114,12) &amp; " in"</f>
         <v>0 ft 10 in</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="I114" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J114">
         <v>77</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -5183,14 +5234,14 @@
         <f>INT(E115/12) &amp; " ft " &amp; MOD(E115,12) &amp; " in"</f>
         <v>1 ft 2 in</v>
       </c>
-      <c r="I115" s="2" t="s">
+      <c r="I115" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J115">
         <v>78</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>103</v>
       </c>
@@ -5216,14 +5267,14 @@
         <f>INT(E116/12) &amp; " ft " &amp; MOD(E116,12) &amp; " in"</f>
         <v>1 ft 6 in</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="I116" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J116">
         <v>79</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -5249,14 +5300,14 @@
         <f>INT(E117/12) &amp; " ft " &amp; MOD(E117,12) &amp; " in"</f>
         <v>1 ft 10 in</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="I117" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J117">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>106</v>
       </c>
@@ -5279,14 +5330,14 @@
         <f>INT(E118/12) &amp; " ft " &amp; MOD(E118,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="I118" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J118">
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>87</v>
       </c>
@@ -5312,11 +5363,17 @@
         <f>INT(E119/12) &amp; " ft " &amp; MOD(E119,12) &amp; " in"</f>
         <v>8 ft 9 in</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="I119" s="1" t="s">
         <v>76</v>
       </c>
       <c r="J119">
         <v>66</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N121">
+        <f>SUM(N2:N119)</f>
+        <v>1263.0999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2x8 board prices
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{ECB15B36-CBF9-4345-A502-0508311F015C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E0E09365-B5EE-A547-AE6E-C5B798F35615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="-21100" windowWidth="29720" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
+    <workbookView xWindow="7300" yWindow="-21100" windowWidth="25200" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_2" sheetId="1" r:id="rId1"/>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O119" sqref="O119"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1582,35 +1582,35 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>78</v>
       </c>
-      <c r="F4">
-        <v>90</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" s="2">
+        <v>90</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="str">
+      <c r="H4" s="2" t="str">
         <f>INT(E4/12) &amp; " ft " &amp; MOD(E4,12) &amp; " in"</f>
         <v>6 ft 6 in</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>17</v>
       </c>
       <c r="K4" s="2"/>
@@ -1623,35 +1623,35 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>77.75</v>
       </c>
-      <c r="F5">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" s="2">
+        <v>90</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="str">
+      <c r="H5" s="2" t="str">
         <f>INT(E5/12) &amp; " ft " &amp; MOD(E5,12) &amp; " in"</f>
         <v>6 ft 5.75 in</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>18</v>
       </c>
       <c r="K5" s="2"/>
@@ -1664,35 +1664,35 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>111</v>
       </c>
-      <c r="F6">
-        <v>90</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" s="2">
+        <v>90</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="str">
+      <c r="H6" s="2" t="str">
         <f>INT(E6/12) &amp; " ft " &amp; MOD(E6,12) &amp; " in"</f>
         <v>9 ft 3 in</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <v>19</v>
       </c>
       <c r="K6" s="2"/>
@@ -1705,35 +1705,35 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>111</v>
       </c>
-      <c r="F7">
-        <v>90</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="2">
+        <v>90</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7" s="2" t="str">
         <f>INT(E7/12) &amp; " ft " &amp; MOD(E7,12) &amp; " in"</f>
         <v>9 ft 3 in</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <v>20</v>
       </c>
       <c r="K7" s="2"/>
@@ -1746,35 +1746,35 @@
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>159</v>
       </c>
-      <c r="F8">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F8" s="2">
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H8" t="str">
+      <c r="H8" s="2" t="str">
         <f>INT(E8/12) &amp; " ft " &amp; MOD(E8,12) &amp; " in"</f>
         <v>13 ft 3 in</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <v>21</v>
       </c>
       <c r="K8" s="2"/>
@@ -1783,35 +1783,35 @@
       <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>144</v>
       </c>
-      <c r="F9">
-        <v>90</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="F9" s="2">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H9" s="2" t="str">
         <f>INT(E9/12) &amp; " ft " &amp; MOD(E9,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <v>22</v>
       </c>
       <c r="K9" s="2"/>
@@ -1820,35 +1820,35 @@
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>52.75</v>
       </c>
-      <c r="F10">
-        <v>90</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="2">
+        <v>90</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H10" t="str">
+      <c r="H10" s="2" t="str">
         <f>INT(E10/12) &amp; " ft " &amp; MOD(E10,12) &amp; " in"</f>
         <v>4 ft 4.75 in</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="2">
         <v>23</v>
       </c>
       <c r="K10" s="2"/>
@@ -1857,35 +1857,35 @@
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>78</v>
       </c>
-      <c r="F11">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" s="2">
+        <v>90</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H11" s="2" t="str">
         <f>INT(E11/12) &amp; " ft " &amp; MOD(E11,12) &amp; " in"</f>
         <v>6 ft 6 in</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>29</v>
       </c>
       <c r="K11" s="2"/>
@@ -1894,32 +1894,33 @@
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>30</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>45</v>
       </c>
-      <c r="H12" t="str">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="str">
         <f>INT(E12/12) &amp; " ft " &amp; MOD(E12,12) &amp; " in"</f>
         <v>2 ft 6 in</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="2">
         <v>30</v>
       </c>
       <c r="K12" s="2"/>
@@ -1961,6 +1962,12 @@
       <c r="J13">
         <v>89</v>
       </c>
+      <c r="L13">
+        <v>168</v>
+      </c>
+      <c r="M13">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1994,6 +2001,12 @@
       <c r="J14">
         <v>90</v>
       </c>
+      <c r="L14">
+        <v>192</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -2027,238 +2040,262 @@
       <c r="J15">
         <v>91</v>
       </c>
+      <c r="N15">
+        <v>148.97999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>96</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>45</v>
       </c>
-      <c r="H16" t="str">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="str">
         <f>INT(E16/12) &amp; " ft " &amp; MOD(E16,12) &amp; " in"</f>
         <v>8 ft 0 in</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
         <v>1</v>
       </c>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="L16" s="2">
+        <v>96</v>
+      </c>
+      <c r="M16" s="2">
+        <v>4</v>
+      </c>
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>120</v>
       </c>
-      <c r="F17">
-        <v>90</v>
-      </c>
-      <c r="H17" t="str">
+      <c r="F17" s="2">
+        <v>90</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="str">
         <f>INT(E17/12) &amp; " ft " &amp; MOD(E17,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="2">
         <v>2</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="L17" s="2">
+        <v>120</v>
+      </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>4</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>120</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>45</v>
       </c>
-      <c r="H18" t="str">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="str">
         <f>INT(E18/12) &amp; " ft " &amp; MOD(E18,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
         <v>3</v>
       </c>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="L18" s="2">
+        <v>144</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>4</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>144</v>
       </c>
-      <c r="F19">
-        <v>90</v>
-      </c>
-      <c r="H19" t="str">
+      <c r="F19" s="2">
+        <v>90</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="str">
         <f>INT(E19/12) &amp; " ft " &amp; MOD(E19,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="2">
         <v>4</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="L19" s="2">
+        <v>168</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>144</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>45</v>
       </c>
-      <c r="H20" t="str">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="str">
         <f>INT(E20/12) &amp; " ft " &amp; MOD(E20,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="2">
         <v>5</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="L20" s="2">
+        <v>192</v>
+      </c>
       <c r="M20" s="3"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>4</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>168</v>
       </c>
-      <c r="F21">
-        <v>90</v>
-      </c>
-      <c r="H21" t="str">
+      <c r="F21" s="2">
+        <v>90</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="str">
         <f>INT(E21/12) &amp; " ft " &amp; MOD(E21,12) &amp; " in"</f>
         <v>14 ft 0 in</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <v>6</v>
       </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2">
+        <v>216</v>
+      </c>
       <c r="M21" s="3"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>168</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>45</v>
       </c>
-      <c r="H22" t="str">
+      <c r="G22" s="2"/>
+      <c r="H22" s="2" t="str">
         <f>INT(E22/12) &amp; " ft " &amp; MOD(E22,12) &amp; " in"</f>
         <v>14 ft 0 in</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <v>7</v>
       </c>
       <c r="K22" s="2"/>
@@ -2267,32 +2304,33 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>192</v>
       </c>
-      <c r="F23">
-        <v>90</v>
-      </c>
-      <c r="H23" t="str">
+      <c r="F23" s="2">
+        <v>90</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="str">
         <f>INT(E23/12) &amp; " ft " &amp; MOD(E23,12) &amp; " in"</f>
         <v>16 ft 0 in</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <v>8</v>
       </c>
       <c r="K23" s="2"/>
@@ -2301,32 +2339,33 @@
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>4</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>144</v>
       </c>
-      <c r="F24">
-        <v>90</v>
-      </c>
-      <c r="H24" t="str">
+      <c r="F24" s="2">
+        <v>90</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="str">
         <f>INT(E24/12) &amp; " ft " &amp; MOD(E24,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <v>9</v>
       </c>
       <c r="K24" s="2"/>
@@ -2335,32 +2374,33 @@
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>21</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>140.5</v>
       </c>
-      <c r="F25">
-        <v>90</v>
-      </c>
-      <c r="H25" t="str">
+      <c r="F25" s="2">
+        <v>90</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2" t="str">
         <f>INT(E25/12) &amp; " ft " &amp; MOD(E25,12) &amp; " in"</f>
         <v>11 ft 8.5 in</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
         <v>10</v>
       </c>
       <c r="K25" s="2"/>
@@ -2369,32 +2409,33 @@
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>34</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>22.13</v>
       </c>
-      <c r="F26">
-        <v>90</v>
-      </c>
-      <c r="H26" t="str">
+      <c r="F26" s="2">
+        <v>90</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2" t="str">
         <f>INT(E26/12) &amp; " ft " &amp; MOD(E26,12) &amp; " in"</f>
         <v>1 ft 10.13 in</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <v>11</v>
       </c>
       <c r="K26" s="2"/>
@@ -2403,32 +2444,33 @@
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>21.25</v>
       </c>
-      <c r="F27">
-        <v>90</v>
-      </c>
-      <c r="H27" t="str">
+      <c r="F27" s="2">
+        <v>90</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2" t="str">
         <f>INT(E27/12) &amp; " ft " &amp; MOD(E27,12) &amp; " in"</f>
         <v>1 ft 9.25 in</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="2">
         <v>12</v>
       </c>
       <c r="K27" s="2"/>
@@ -2437,35 +2479,35 @@
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>42</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>75.38</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>18.5</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H28" t="str">
+      <c r="H28" s="2" t="str">
         <f>INT(E28/12) &amp; " ft " &amp; MOD(E28,12) &amp; " in"</f>
         <v>6 ft 3.38 in</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="2">
         <v>84</v>
       </c>
       <c r="K28" s="2"/>
@@ -2598,7 +2640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2628,7 +2670,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2661,7 +2703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2691,7 +2733,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2721,7 +2763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2754,166 +2796,178 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
         <v>28</v>
       </c>
       <c r="E38">
-        <v>192</v>
+        <v>12</v>
       </c>
       <c r="F38">
         <v>90</v>
-      </c>
-      <c r="G38" t="s">
-        <v>125</v>
       </c>
       <c r="H38" t="str">
         <f>INT(E38/12) &amp; " ft " &amp; MOD(E38,12) &amp; " in"</f>
-        <v>16 ft 0 in</v>
+        <v>1 ft 0 in</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="J38">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>28</v>
       </c>
       <c r="E39">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="F39">
         <v>90</v>
-      </c>
-      <c r="G39" t="s">
-        <v>125</v>
       </c>
       <c r="H39" t="str">
         <f>INT(E39/12) &amp; " ft " &amp; MOD(E39,12) &amp; " in"</f>
+        <v>12 ft 0 in</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="2">
+        <v>192</v>
+      </c>
+      <c r="F40" s="2">
+        <v>90</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" s="2" t="str">
+        <f>INT(E40/12) &amp; " ft " &amp; MOD(E40,12) &amp; " in"</f>
+        <v>16 ft 0 in</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J40" s="2">
+        <v>92</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="2">
+        <v>120</v>
+      </c>
+      <c r="F41" s="2">
+        <v>90</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" s="2" t="str">
+        <f>INT(E41/12) &amp; " ft " &amp; MOD(E41,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I41" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J39">
+      <c r="J41" s="2">
         <v>93</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40">
+      <c r="B42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="2">
         <v>4</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D42" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E40">
+      <c r="E42" s="2">
         <v>83</v>
       </c>
-      <c r="F40">
+      <c r="F42" s="2">
         <v>18.5</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G42" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H40" t="str">
-        <f>INT(E40/12) &amp; " ft " &amp; MOD(E40,12) &amp; " in"</f>
+      <c r="H42" s="2" t="str">
+        <f>INT(E42/12) &amp; " ft " &amp; MOD(E42,12) &amp; " in"</f>
         <v>6 ft 11 in</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I42" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J40">
+      <c r="J42" s="2">
         <v>94</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>158</v>
-      </c>
-      <c r="B41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41">
-        <v>12</v>
-      </c>
-      <c r="F41">
-        <v>90</v>
-      </c>
-      <c r="H41" t="str">
-        <f>INT(E41/12) &amp; " ft " &amp; MOD(E41,12) &amp; " in"</f>
-        <v>1 ft 0 in</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J41">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>159</v>
-      </c>
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
-        <v>28</v>
-      </c>
-      <c r="E42">
-        <v>144</v>
-      </c>
-      <c r="F42">
-        <v>90</v>
-      </c>
-      <c r="H42" t="str">
-        <f>INT(E42/12) &amp; " ft " &amp; MOD(E42,12) &amp; " in"</f>
-        <v>12 ft 0 in</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J42">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>173</v>
       </c>
@@ -2943,7 +2997,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2973,7 +3027,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3003,7 +3057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -3036,7 +3090,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3069,7 +3123,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>172</v>
       </c>
@@ -5373,7 +5427,7 @@
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N121">
         <f>SUM(N2:N119)</f>
-        <v>1263.0999999999999</v>
+        <v>1412.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plywood prices to bom
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D97FB739-ADD5-E642-801E-7686B19B71A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F281741-EB62-6147-A4F3-2F2412BBD517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3580" yWindow="-21100" windowWidth="37880" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="586" uniqueCount="188">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="587" uniqueCount="189">
   <si>
     <t>FLOOR</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>Subtotal</t>
+  </si>
+  <si>
+    <t>https://www.hepsales.com/cdx-plywood-3-4-in-x-4-ft-x-8-ft-pine/</t>
   </si>
 </sst>
 </file>
@@ -1489,8 +1492,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0679CAE-7790-0146-A436-E7EEAE9C9294}">
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1506,7 +1509,7 @@
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="55.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -1587,6 +1590,26 @@
       <c r="J2">
         <v>15</v>
       </c>
+      <c r="L2">
+        <v>96</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>INT(L2/12) &amp; " ft "</f>
+        <v xml:space="preserve">8 ft </v>
+      </c>
+      <c r="N2">
+        <v>14</v>
+      </c>
+      <c r="O2">
+        <v>41.77</v>
+      </c>
+      <c r="P2">
+        <f>O2*N2</f>
+        <v>584.78000000000009</v>
+      </c>
+      <c r="R2" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1616,6 +1639,10 @@
       </c>
       <c r="J3">
         <v>16</v>
+      </c>
+      <c r="Q3">
+        <f>P2</f>
+        <v>584.78000000000009</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -5936,7 +5963,7 @@
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P120">
         <f>SUM(P2:P119)</f>
-        <v>1603.7700000000002</v>
+        <v>2188.5499999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 1x8 board prices
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0F281741-EB62-6147-A4F3-2F2412BBD517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4BD9E0E8-60E2-F149-95D1-44F2BCD2EE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3580" yWindow="-21100" windowWidth="37880" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
+    <workbookView xWindow="7000" yWindow="-21100" windowWidth="27100" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="587" uniqueCount="189">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="591" uniqueCount="189">
   <si>
     <t>FLOOR</t>
   </si>
@@ -1492,8 +1492,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0679CAE-7790-0146-A436-E7EEAE9C9294}">
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="G33" workbookViewId="0">
+      <selection activeCell="P69" sqref="P69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3353,7 +3353,7 @@
         <v>168</v>
       </c>
       <c r="M41" s="3" t="str">
-        <f t="shared" ref="M41:M42" si="6">INT(L41/12) &amp; " ft "</f>
+        <f t="shared" ref="M41:M46" si="6">INT(L41/12) &amp; " ft "</f>
         <v xml:space="preserve">14 ft </v>
       </c>
       <c r="N41" s="3">
@@ -3457,6 +3457,29 @@
       </c>
       <c r="J43">
         <v>13</v>
+      </c>
+      <c r="L43" s="2">
+        <v>120</v>
+      </c>
+      <c r="M43" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">10 ft </v>
+      </c>
+      <c r="N43" s="2">
+        <v>1</v>
+      </c>
+      <c r="O43" s="2">
+        <v>6</v>
+      </c>
+      <c r="P43" s="2">
+        <f>O43*N43</f>
+        <v>6</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>6</v>
+      </c>
+      <c r="R43" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
@@ -3490,12 +3513,27 @@
         <v>38</v>
       </c>
       <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
+      <c r="L44" s="3">
+        <v>96</v>
+      </c>
+      <c r="M44" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">8 ft </v>
+      </c>
+      <c r="N44" s="3">
+        <v>5</v>
+      </c>
+      <c r="O44" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="P44" s="3">
+        <f>O44*N44</f>
+        <v>24</v>
+      </c>
       <c r="Q44" s="3"/>
+      <c r="R44" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -3528,12 +3566,27 @@
         <v>40</v>
       </c>
       <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
+      <c r="L45" s="3">
+        <v>144</v>
+      </c>
+      <c r="M45" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">12 ft </v>
+      </c>
+      <c r="N45" s="3">
+        <v>1</v>
+      </c>
+      <c r="O45" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="P45" s="3">
+        <f>O45*N45</f>
+        <v>7.6</v>
+      </c>
       <c r="Q45" s="3"/>
+      <c r="R45" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
@@ -3568,12 +3621,27 @@
         <v>82</v>
       </c>
       <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
+      <c r="L46" s="3">
+        <v>168</v>
+      </c>
+      <c r="M46" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">14 ft </v>
+      </c>
+      <c r="N46" s="3">
+        <v>2</v>
+      </c>
+      <c r="O46" s="3">
+        <v>8.86</v>
+      </c>
+      <c r="P46" s="3">
+        <f>O46*N46</f>
+        <v>17.72</v>
+      </c>
       <c r="Q46" s="3"/>
+      <c r="R46" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
@@ -3613,7 +3681,10 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
+      <c r="Q47" s="3">
+        <f>SUM(P44:P46)</f>
+        <v>49.32</v>
+      </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -5963,7 +6034,7 @@
     <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P120">
         <f>SUM(P2:P119)</f>
-        <v>2188.5499999999997</v>
+        <v>2243.8699999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 1x6 board prices
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4BD9E0E8-60E2-F149-95D1-44F2BCD2EE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F01C4DCA-BBEE-9B4F-9241-7D6B1ED76A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7000" yWindow="-21100" windowWidth="27100" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
+    <workbookView xWindow="5520" yWindow="-21100" windowWidth="27420" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="591" uniqueCount="189">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="594" uniqueCount="189">
   <si>
     <t>FLOOR</t>
   </si>
@@ -1490,10 +1490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0679CAE-7790-0146-A436-E7EEAE9C9294}">
-  <dimension ref="A1:R120"/>
+  <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G33" workbookViewId="0">
-      <selection activeCell="P69" sqref="P69"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3353,7 +3353,7 @@
         <v>168</v>
       </c>
       <c r="M41" s="3" t="str">
-        <f t="shared" ref="M41:M46" si="6">INT(L41/12) &amp; " ft "</f>
+        <f t="shared" ref="M41:M52" si="6">INT(L41/12) &amp; " ft "</f>
         <v xml:space="preserve">14 ft </v>
       </c>
       <c r="N41" s="3">
@@ -3717,565 +3717,671 @@
         <v>14</v>
       </c>
       <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
+      <c r="L48" s="2">
+        <v>120</v>
+      </c>
+      <c r="M48" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">10 ft </v>
+      </c>
+      <c r="N48" s="2">
+        <v>1</v>
+      </c>
+      <c r="O48" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="P48" s="2">
+        <f>O48*N48</f>
+        <v>4.5</v>
+      </c>
       <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E49" s="2">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F49" s="2">
-        <v>18.5</v>
+        <v>71.5</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="H49" s="2" t="str">
         <f>INT(E49/12) &amp; " ft " &amp; MOD(E49,12) &amp; " in"</f>
+        <v>6 ft 10 in</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J49" s="2">
+        <v>85</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2">
+        <v>168</v>
+      </c>
+      <c r="M49" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">14 ft </v>
+      </c>
+      <c r="N49" s="2">
+        <v>5</v>
+      </c>
+      <c r="O49" s="2">
+        <v>6.65</v>
+      </c>
+      <c r="P49" s="2">
+        <f t="shared" ref="P49:P52" si="8">O49*N49</f>
+        <v>33.25</v>
+      </c>
+      <c r="Q49" s="2"/>
+      <c r="R49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2">
+        <v>192</v>
+      </c>
+      <c r="M50" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">16 ft </v>
+      </c>
+      <c r="N50" s="2">
+        <v>9</v>
+      </c>
+      <c r="O50" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="P50" s="2">
+        <f t="shared" si="8"/>
+        <v>68.399999999999991</v>
+      </c>
+      <c r="Q50" s="2">
+        <f>SUM(P48:P50)</f>
+        <v>106.14999999999999</v>
+      </c>
+      <c r="R50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="3">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="3">
+        <v>90</v>
+      </c>
+      <c r="F51" s="3">
+        <v>18.5</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H51" s="3" t="str">
+        <f>INT(E51/12) &amp; " ft " &amp; MOD(E51,12) &amp; " in"</f>
         <v>7 ft 6 in</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I51" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J51" s="3">
         <v>47</v>
       </c>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="2">
-        <v>17</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="K51" s="3"/>
+      <c r="L51" s="3">
+        <v>96</v>
+      </c>
+      <c r="M51" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">8 ft </v>
+      </c>
+      <c r="N51" s="3">
+        <v>1</v>
+      </c>
+      <c r="O51" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="P51" s="3">
+        <f t="shared" si="8"/>
+        <v>3.6</v>
+      </c>
+      <c r="Q51" s="3"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="2">
-        <v>82</v>
-      </c>
-      <c r="F50" s="2">
-        <v>71.5</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H50" s="2" t="str">
-        <f>INT(E50/12) &amp; " ft " &amp; MOD(E50,12) &amp; " in"</f>
-        <v>6 ft 10 in</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J50" s="2">
-        <v>85</v>
-      </c>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="2">
+      <c r="E52" s="3">
+        <v>75.38</v>
+      </c>
+      <c r="F52" s="3">
+        <v>18.5</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H52" s="3" t="str">
+        <f>INT(E52/12) &amp; " ft " &amp; MOD(E52,12) &amp; " in"</f>
+        <v>6 ft 3.38 in</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J52" s="3">
+        <v>109</v>
+      </c>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3">
+        <v>168</v>
+      </c>
+      <c r="M52" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">14 ft </v>
+      </c>
+      <c r="N52" s="3">
+        <v>3</v>
+      </c>
+      <c r="O52" s="3">
+        <v>6.65</v>
+      </c>
+      <c r="P52" s="3">
+        <f t="shared" si="8"/>
+        <v>19.950000000000003</v>
+      </c>
+      <c r="Q52" s="3"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="3">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="3">
+        <v>147</v>
+      </c>
+      <c r="F53" s="3">
+        <v>90</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H53" s="3" t="str">
+        <f>INT(E53/12) &amp; " ft " &amp; MOD(E53,12) &amp; " in"</f>
+        <v>12 ft 3 in</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J53" s="3">
+        <v>110</v>
+      </c>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="3">
         <v>2</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D54" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E51" s="2">
-        <v>75.38</v>
-      </c>
-      <c r="F51" s="2">
-        <v>18.5</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H51" s="2" t="str">
-        <f>INT(E51/12) &amp; " ft " &amp; MOD(E51,12) &amp; " in"</f>
-        <v>6 ft 3.38 in</v>
-      </c>
-      <c r="I51" s="2" t="s">
+      <c r="E54" s="3">
+        <v>48</v>
+      </c>
+      <c r="F54" s="3">
+        <v>90</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3" t="str">
+        <f>INT(E54/12) &amp; " ft " &amp; MOD(E54,12) &amp; " in"</f>
+        <v>4 ft 0 in</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J51" s="2">
-        <v>109</v>
-      </c>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E52" s="2">
-        <v>147</v>
-      </c>
-      <c r="F52" s="2">
-        <v>90</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H52" s="2" t="str">
-        <f>INT(E52/12) &amp; " ft " &amp; MOD(E52,12) &amp; " in"</f>
-        <v>12 ft 3 in</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J52" s="2">
-        <v>110</v>
-      </c>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" s="2">
+      <c r="J54" s="3">
+        <v>111</v>
+      </c>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3">
+        <f>SUM(P51:P52)</f>
+        <v>23.550000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55">
         <v>2</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" s="2">
-        <v>48</v>
-      </c>
-      <c r="F53" s="2">
-        <v>90</v>
-      </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2" t="str">
-        <f>INT(E53/12) &amp; " ft " &amp; MOD(E53,12) &amp; " in"</f>
-        <v>4 ft 0 in</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J53" s="2">
-        <v>111</v>
-      </c>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>135</v>
-      </c>
-      <c r="B54" t="s">
-        <v>51</v>
-      </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54" t="s">
-        <v>136</v>
-      </c>
-      <c r="E54">
-        <v>80</v>
-      </c>
-      <c r="F54">
-        <v>90</v>
-      </c>
-      <c r="H54" t="str">
-        <f>INT(E54/12) &amp; " ft " &amp; MOD(E54,12) &amp; " in"</f>
-        <v>6 ft 8 in</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J54">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>138</v>
-      </c>
-      <c r="B55" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
       </c>
       <c r="D55" t="s">
         <v>136</v>
       </c>
       <c r="E55">
-        <v>38.5</v>
+        <v>80</v>
       </c>
       <c r="F55">
         <v>90</v>
-      </c>
-      <c r="G55" t="s">
-        <v>60</v>
       </c>
       <c r="H55" t="str">
         <f>INT(E55/12) &amp; " ft " &amp; MOD(E55,12) &amp; " in"</f>
-        <v>3 ft 2.5 in</v>
+        <v>6 ft 8 in</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>139</v>
       </c>
       <c r="J55">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
         <v>51</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
         <v>136</v>
       </c>
       <c r="E56">
-        <v>81</v>
+        <v>38.5</v>
       </c>
       <c r="F56">
         <v>90</v>
+      </c>
+      <c r="G56" t="s">
+        <v>60</v>
       </c>
       <c r="H56" t="str">
         <f>INT(E56/12) &amp; " ft " &amp; MOD(E56,12) &amp; " in"</f>
-        <v>6 ft 9 in</v>
+        <v>3 ft 2.5 in</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>139</v>
       </c>
       <c r="J56">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C57">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="E57">
-        <v>192</v>
+        <v>81</v>
       </c>
       <c r="F57">
         <v>90</v>
-      </c>
-      <c r="G57" t="s">
-        <v>120</v>
       </c>
       <c r="H57" t="str">
         <f>INT(E57/12) &amp; " ft " &amp; MOD(E57,12) &amp; " in"</f>
+        <v>6 ft 9 in</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J57">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="3">
+        <v>10</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="3">
+        <v>192</v>
+      </c>
+      <c r="F58" s="3">
+        <v>90</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H58" s="3" t="str">
+        <f>INT(E58/12) &amp; " ft " &amp; MOD(E58,12) &amp; " in"</f>
         <v>16 ft 0 in</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="I58" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J57">
+      <c r="J58" s="3">
         <v>86</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C58">
+      <c r="C59" s="3">
         <v>20</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E58">
+      <c r="E59" s="3">
         <v>120</v>
       </c>
-      <c r="F58">
-        <v>90</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="F59" s="3">
+        <v>90</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="H58" t="str">
-        <f>INT(E58/12) &amp; " ft " &amp; MOD(E58,12) &amp; " in"</f>
+      <c r="H59" s="3" t="str">
+        <f>INT(E59/12) &amp; " ft " &amp; MOD(E59,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="I59" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J58">
+      <c r="J59" s="3">
         <v>87</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C59">
+      <c r="C60" s="3">
         <v>10</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E59">
+      <c r="E60" s="3">
         <v>46</v>
       </c>
-      <c r="F59">
-        <v>90</v>
-      </c>
-      <c r="H59" t="str">
-        <f>INT(E59/12) &amp; " ft " &amp; MOD(E59,12) &amp; " in"</f>
+      <c r="F60" s="3">
+        <v>90</v>
+      </c>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3" t="str">
+        <f>INT(E60/12) &amp; " ft " &amp; MOD(E60,12) &amp; " in"</f>
         <v>3 ft 10 in</v>
       </c>
-      <c r="I59" s="2" t="s">
+      <c r="I60" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J59">
+      <c r="J60" s="3">
         <v>88</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" s="3">
+        <v>120</v>
+      </c>
+      <c r="F61" s="3">
+        <v>90</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3" t="str">
+        <f>INT(E61/12) &amp; " ft " &amp; MOD(E61,12) &amp; " in"</f>
+        <v>10 ft 0 in</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J61" s="3">
+        <v>112</v>
+      </c>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="3">
+        <v>6</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E62" s="3">
+        <v>144</v>
+      </c>
+      <c r="F62" s="3">
+        <v>90</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3" t="str">
+        <f>INT(E62/12) &amp; " ft " &amp; MOD(E62,12) &amp; " in"</f>
+        <v>12 ft 0 in</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J62" s="3">
+        <v>113</v>
+      </c>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="3">
+        <v>3</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" s="3">
+        <v>168</v>
+      </c>
+      <c r="F63" s="3">
+        <v>90</v>
+      </c>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3" t="str">
+        <f>INT(E63/12) &amp; " ft " &amp; MOD(E63,12) &amp; " in"</f>
+        <v>14 ft 0 in</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J63" s="3">
+        <v>114</v>
+      </c>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E64" s="3">
+        <v>48</v>
+      </c>
+      <c r="F64" s="3">
+        <v>90</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3" t="str">
+        <f>INT(E64/12) &amp; " ft " &amp; MOD(E64,12) &amp; " in"</f>
+        <v>4 ft 0 in</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J64" s="3">
+        <v>115</v>
+      </c>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>134</v>
-      </c>
-      <c r="B60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60">
-        <v>4</v>
-      </c>
-      <c r="D60" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60">
-        <v>88</v>
-      </c>
-      <c r="F60">
-        <v>90</v>
-      </c>
-      <c r="G60" t="s">
-        <v>130</v>
-      </c>
-      <c r="H60" t="str">
-        <f>INT(E60/12) &amp; " ft " &amp; MOD(E60,12) &amp; " in"</f>
-        <v>7 ft 4 in</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J60">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>137</v>
-      </c>
-      <c r="B61" t="s">
-        <v>51</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
-        <v>119</v>
-      </c>
-      <c r="E61">
-        <v>90</v>
-      </c>
-      <c r="F61">
-        <v>18.5</v>
-      </c>
-      <c r="G61" t="s">
-        <v>60</v>
-      </c>
-      <c r="H61" t="str">
-        <f>INT(E61/12) &amp; " ft " &amp; MOD(E61,12) &amp; " in"</f>
-        <v>7 ft 6 in</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J61">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>141</v>
-      </c>
-      <c r="B62" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62" t="s">
-        <v>119</v>
-      </c>
-      <c r="E62">
-        <v>44.5</v>
-      </c>
-      <c r="F62">
-        <v>90</v>
-      </c>
-      <c r="G62" t="s">
-        <v>142</v>
-      </c>
-      <c r="H62" t="str">
-        <f>INT(E62/12) &amp; " ft " &amp; MOD(E62,12) &amp; " in"</f>
-        <v>3 ft 8.5 in</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J62">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>143</v>
-      </c>
-      <c r="B63" t="s">
-        <v>51</v>
-      </c>
-      <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63">
-        <v>81</v>
-      </c>
-      <c r="F63">
-        <v>90</v>
-      </c>
-      <c r="G63" t="s">
-        <v>142</v>
-      </c>
-      <c r="H63" t="str">
-        <f>INT(E63/12) &amp; " ft " &amp; MOD(E63,12) &amp; " in"</f>
-        <v>6 ft 9 in</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J63">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>147</v>
-      </c>
-      <c r="B64" t="s">
-        <v>51</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
-      </c>
-      <c r="D64" t="s">
-        <v>119</v>
-      </c>
-      <c r="E64">
-        <v>44.5</v>
-      </c>
-      <c r="F64">
-        <v>90</v>
-      </c>
-      <c r="H64" t="str">
-        <f>INT(E64/12) &amp; " ft " &amp; MOD(E64,12) &amp; " in"</f>
-        <v>3 ft 8.5 in</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J64">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>148</v>
       </c>
       <c r="B65" t="s">
         <v>51</v>
@@ -4287,145 +4393,157 @@
         <v>119</v>
       </c>
       <c r="E65">
-        <v>24.5</v>
+        <v>88</v>
       </c>
       <c r="F65">
         <v>90</v>
+      </c>
+      <c r="G65" t="s">
+        <v>130</v>
       </c>
       <c r="H65" t="str">
         <f>INT(E65/12) &amp; " ft " &amp; MOD(E65,12) &amp; " in"</f>
-        <v>2 ft 0.5 in</v>
+        <v>7 ft 4 in</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>139</v>
       </c>
       <c r="J65">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D66" t="s">
         <v>119</v>
       </c>
       <c r="E66">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="F66">
-        <v>90</v>
+        <v>18.5</v>
+      </c>
+      <c r="G66" t="s">
+        <v>60</v>
       </c>
       <c r="H66" t="str">
         <f>INT(E66/12) &amp; " ft " &amp; MOD(E66,12) &amp; " in"</f>
-        <v>10 ft 0 in</v>
+        <v>7 ft 6 in</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="J66">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C67">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
         <v>119</v>
       </c>
       <c r="E67">
-        <v>144</v>
+        <v>44.5</v>
       </c>
       <c r="F67">
         <v>90</v>
+      </c>
+      <c r="G67" t="s">
+        <v>142</v>
       </c>
       <c r="H67" t="str">
         <f>INT(E67/12) &amp; " ft " &amp; MOD(E67,12) &amp; " in"</f>
-        <v>12 ft 0 in</v>
+        <v>3 ft 8.5 in</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="J67">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D68" t="s">
         <v>119</v>
       </c>
       <c r="E68">
-        <v>168</v>
+        <v>81</v>
       </c>
       <c r="F68">
         <v>90</v>
+      </c>
+      <c r="G68" t="s">
+        <v>142</v>
       </c>
       <c r="H68" t="str">
         <f>INT(E68/12) &amp; " ft " &amp; MOD(E68,12) &amp; " in"</f>
-        <v>14 ft 0 in</v>
+        <v>6 ft 9 in</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="J68">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D69" t="s">
         <v>119</v>
       </c>
       <c r="E69">
-        <v>48</v>
+        <v>44.5</v>
       </c>
       <c r="F69">
         <v>90</v>
       </c>
       <c r="H69" t="str">
         <f>INT(E69/12) &amp; " ft " &amp; MOD(E69,12) &amp; " in"</f>
-        <v>4 ft 0 in</v>
+        <v>3 ft 8.5 in</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="J69">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B70" t="s">
         <v>51</v>
@@ -4434,829 +4552,996 @@
         <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="E70">
-        <v>36.5</v>
+        <v>24.5</v>
       </c>
       <c r="F70">
         <v>90</v>
       </c>
       <c r="H70" t="str">
         <f>INT(E70/12) &amp; " ft " &amp; MOD(E70,12) &amp; " in"</f>
-        <v>3 ft 0.5 in</v>
+        <v>2 ft 0.5 in</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>139</v>
       </c>
       <c r="J70">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="3">
+        <v>4</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E71" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="F71" s="3">
+        <v>90</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3" t="str">
+        <f>INT(E71/12) &amp; " ft " &amp; MOD(E71,12) &amp; " in"</f>
+        <v>3 ft 0.5 in</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J71" s="3">
         <v>106</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B71" t="s">
-        <v>51</v>
-      </c>
-      <c r="C71">
+      <c r="B72" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="3">
         <v>4</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E71">
+      <c r="E72" s="3">
         <v>22.5</v>
       </c>
-      <c r="F71">
-        <v>90</v>
-      </c>
-      <c r="H71" t="str">
-        <f>INT(E71/12) &amp; " ft " &amp; MOD(E71,12) &amp; " in"</f>
+      <c r="F72" s="3">
+        <v>90</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3" t="str">
+        <f>INT(E72/12) &amp; " ft " &amp; MOD(E72,12) &amp; " in"</f>
         <v>1 ft 10.5 in</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I72" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J71">
+      <c r="J72" s="3">
         <v>107</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B72" t="s">
-        <v>51</v>
-      </c>
-      <c r="C72">
+      <c r="B73" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73" s="3">
         <v>2</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E72">
+      <c r="E73" s="3">
         <v>75.38</v>
       </c>
-      <c r="F72">
+      <c r="F73" s="3">
         <v>18.5</v>
       </c>
-      <c r="G72" t="s">
+      <c r="G73" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H72" t="str">
-        <f>INT(E72/12) &amp; " ft " &amp; MOD(E72,12) &amp; " in"</f>
+      <c r="H73" s="3" t="str">
+        <f>INT(E73/12) &amp; " ft " &amp; MOD(E73,12) &amp; " in"</f>
         <v>6 ft 3.38 in</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="I73" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J72">
+      <c r="J73" s="3">
         <v>108</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>144</v>
       </c>
-      <c r="B73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C73">
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74">
         <v>1</v>
-      </c>
-      <c r="D73" t="s">
-        <v>145</v>
-      </c>
-      <c r="E73">
-        <v>36.5</v>
-      </c>
-      <c r="F73">
-        <v>90</v>
-      </c>
-      <c r="H73" t="str">
-        <f>INT(E73/12) &amp; " ft " &amp; MOD(E73,12) &amp; " in"</f>
-        <v>3 ft 0.5 in</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J73">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>146</v>
-      </c>
-      <c r="B74" t="s">
-        <v>51</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
       </c>
       <c r="D74" t="s">
         <v>145</v>
       </c>
       <c r="E74">
-        <v>80</v>
+        <v>36.5</v>
       </c>
       <c r="F74">
         <v>90</v>
       </c>
       <c r="H74" t="str">
         <f>INT(E74/12) &amp; " ft " &amp; MOD(E74,12) &amp; " in"</f>
-        <v>6 ft 8 in</v>
+        <v>3 ft 0.5 in</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>139</v>
       </c>
       <c r="J74">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="B75" t="s">
         <v>51</v>
       </c>
       <c r="C75">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="E75">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F75">
         <v>90</v>
       </c>
       <c r="H75" t="str">
         <f>INT(E75/12) &amp; " ft " &amp; MOD(E75,12) &amp; " in"</f>
+        <v>6 ft 8 in</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J75">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="3">
+        <v>65</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E76" s="3">
+        <v>93</v>
+      </c>
+      <c r="F76" s="3">
+        <v>90</v>
+      </c>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3" t="str">
+        <f>INT(E76/12) &amp; " ft " &amp; MOD(E76,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="I76" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J75">
+      <c r="J76" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B76" t="s">
-        <v>51</v>
-      </c>
-      <c r="C76">
+      <c r="B77" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" s="3">
         <v>6</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E76">
+      <c r="E77" s="3">
         <v>49</v>
       </c>
-      <c r="F76">
-        <v>90</v>
-      </c>
-      <c r="H76" t="str">
-        <f>INT(E76/12) &amp; " ft " &amp; MOD(E76,12) &amp; " in"</f>
+      <c r="F77" s="3">
+        <v>90</v>
+      </c>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3" t="str">
+        <f>INT(E77/12) &amp; " ft " &amp; MOD(E77,12) &amp; " in"</f>
         <v>4 ft 1 in</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="I77" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J76">
+      <c r="J77" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B77" t="s">
-        <v>51</v>
-      </c>
-      <c r="C77">
+      <c r="B78" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="3">
         <v>6</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E77">
+      <c r="E78" s="3">
         <v>20</v>
       </c>
-      <c r="F77">
-        <v>90</v>
-      </c>
-      <c r="H77" t="str">
-        <f>INT(E77/12) &amp; " ft " &amp; MOD(E77,12) &amp; " in"</f>
+      <c r="F78" s="3">
+        <v>90</v>
+      </c>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3" t="str">
+        <f>INT(E78/12) &amp; " ft " &amp; MOD(E78,12) &amp; " in"</f>
         <v>1 ft 8 in</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="I78" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J77">
+      <c r="J78" s="3">
         <v>37</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B78" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78">
+      <c r="B79" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="3">
         <v>2</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E78">
+      <c r="E79" s="3">
         <v>100</v>
       </c>
-      <c r="F78">
+      <c r="F79" s="3">
         <v>18.5</v>
       </c>
-      <c r="G78" t="s">
+      <c r="G79" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H78" t="str">
-        <f>INT(E78/12) &amp; " ft " &amp; MOD(E78,12) &amp; " in"</f>
+      <c r="H79" s="3" t="str">
+        <f>INT(E79/12) &amp; " ft " &amp; MOD(E79,12) &amp; " in"</f>
         <v>8 ft 4 in</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I79" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J78">
+      <c r="J79" s="3">
         <v>41</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B79" t="s">
-        <v>51</v>
-      </c>
-      <c r="C79">
+      <c r="B80" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="3">
         <v>2</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E79">
+      <c r="E80" s="3">
         <v>104</v>
       </c>
-      <c r="F79">
+      <c r="F80" s="3">
         <v>18.5</v>
       </c>
-      <c r="G79" t="s">
+      <c r="G80" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H79" t="str">
-        <f>INT(E79/12) &amp; " ft " &amp; MOD(E79,12) &amp; " in"</f>
+      <c r="H80" s="3" t="str">
+        <f>INT(E80/12) &amp; " ft " &amp; MOD(E80,12) &amp; " in"</f>
         <v>8 ft 8 in</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="I80" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J79">
+      <c r="J80" s="3">
         <v>42</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B80" t="s">
-        <v>51</v>
-      </c>
-      <c r="C80">
+      <c r="B81" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C81" s="3">
         <v>2</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D81" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E80">
+      <c r="E81" s="3">
         <v>108</v>
       </c>
-      <c r="F80">
+      <c r="F81" s="3">
         <v>18.5</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G81" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H80" t="str">
-        <f>INT(E80/12) &amp; " ft " &amp; MOD(E80,12) &amp; " in"</f>
+      <c r="H81" s="3" t="str">
+        <f>INT(E81/12) &amp; " ft " &amp; MOD(E81,12) &amp; " in"</f>
         <v>9 ft 0 in</v>
       </c>
-      <c r="I80" s="2" t="s">
+      <c r="I81" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J80">
+      <c r="J81" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B81" t="s">
-        <v>51</v>
-      </c>
-      <c r="C81">
+      <c r="B82" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C82" s="3">
         <v>2</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D82" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E81">
+      <c r="E82" s="3">
         <v>112</v>
       </c>
-      <c r="F81">
+      <c r="F82" s="3">
         <v>18.5</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H81" t="str">
-        <f>INT(E81/12) &amp; " ft " &amp; MOD(E81,12) &amp; " in"</f>
+      <c r="H82" s="3" t="str">
+        <f>INT(E82/12) &amp; " ft " &amp; MOD(E82,12) &amp; " in"</f>
         <v>9 ft 4 in</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="I82" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J81">
+      <c r="J82" s="3">
         <v>44</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B82" t="s">
-        <v>51</v>
-      </c>
-      <c r="C82">
+      <c r="B83" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C83" s="3">
         <v>2</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E82">
+      <c r="E83" s="3">
         <v>116</v>
       </c>
-      <c r="F82">
+      <c r="F83" s="3">
         <v>18.5</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G83" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H82" t="str">
-        <f>INT(E82/12) &amp; " ft " &amp; MOD(E82,12) &amp; " in"</f>
+      <c r="H83" s="3" t="str">
+        <f>INT(E83/12) &amp; " ft " &amp; MOD(E83,12) &amp; " in"</f>
         <v>9 ft 8 in</v>
       </c>
-      <c r="I82" s="2" t="s">
+      <c r="I83" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J82">
+      <c r="J83" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B83" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83">
+      <c r="B84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C84" s="3">
         <v>2</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E83">
+      <c r="E84" s="3">
         <v>120</v>
       </c>
-      <c r="F83">
+      <c r="F84" s="3">
         <v>18.5</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G84" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H83" t="str">
-        <f>INT(E83/12) &amp; " ft " &amp; MOD(E83,12) &amp; " in"</f>
+      <c r="H84" s="3" t="str">
+        <f>INT(E84/12) &amp; " ft " &amp; MOD(E84,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="I84" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J83">
+      <c r="J84" s="3">
         <v>46</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B84" t="s">
-        <v>51</v>
-      </c>
-      <c r="C84">
+      <c r="B85" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" s="3">
         <v>2</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D85" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E84">
+      <c r="E85" s="3">
         <v>94</v>
       </c>
-      <c r="F84">
+      <c r="F85" s="3">
         <v>18.5</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G85" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H84" t="str">
-        <f>INT(E84/12) &amp; " ft " &amp; MOD(E84,12) &amp; " in"</f>
+      <c r="H85" s="3" t="str">
+        <f>INT(E85/12) &amp; " ft " &amp; MOD(E85,12) &amp; " in"</f>
         <v>7 ft 10 in</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I85" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J84">
+      <c r="J85" s="3">
         <v>48</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B85" t="s">
-        <v>51</v>
-      </c>
-      <c r="C85">
+      <c r="B86" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C86" s="3">
         <v>2</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E85">
+      <c r="E86" s="3">
         <v>98</v>
       </c>
-      <c r="F85">
+      <c r="F86" s="3">
         <v>18.5</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G86" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H85" t="str">
-        <f>INT(E85/12) &amp; " ft " &amp; MOD(E85,12) &amp; " in"</f>
+      <c r="H86" s="3" t="str">
+        <f>INT(E86/12) &amp; " ft " &amp; MOD(E86,12) &amp; " in"</f>
         <v>8 ft 2 in</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I86" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J85">
+      <c r="J86" s="3">
         <v>49</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B86" t="s">
-        <v>51</v>
-      </c>
-      <c r="C86">
+      <c r="B87" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C87" s="3">
         <v>2</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D87" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E86">
+      <c r="E87" s="3">
         <v>106</v>
       </c>
-      <c r="F86">
+      <c r="F87" s="3">
         <v>18.5</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H86" t="str">
-        <f>INT(E86/12) &amp; " ft " &amp; MOD(E86,12) &amp; " in"</f>
+      <c r="H87" s="3" t="str">
+        <f>INT(E87/12) &amp; " ft " &amp; MOD(E87,12) &amp; " in"</f>
         <v>8 ft 10 in</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I87" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J86">
+      <c r="J87" s="3">
         <v>50</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="K87" s="3"/>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B87" t="s">
-        <v>51</v>
-      </c>
-      <c r="C87">
+      <c r="B88" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C88" s="3">
         <v>2</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E87">
+      <c r="E88" s="3">
         <v>102</v>
       </c>
-      <c r="F87">
+      <c r="F88" s="3">
         <v>18.5</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H87" t="str">
-        <f>INT(E87/12) &amp; " ft " &amp; MOD(E87,12) &amp; " in"</f>
+      <c r="H88" s="3" t="str">
+        <f>INT(E88/12) &amp; " ft " &amp; MOD(E88,12) &amp; " in"</f>
         <v>8 ft 6 in</v>
       </c>
-      <c r="I87" s="2" t="s">
+      <c r="I88" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J87">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="J88" s="3">
+        <v>51</v>
+      </c>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B88" t="s">
-        <v>51</v>
-      </c>
-      <c r="C88">
+      <c r="B89" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C89" s="3">
         <v>2</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E88">
+      <c r="E89" s="3">
         <v>28.25</v>
       </c>
-      <c r="F88">
+      <c r="F89" s="3">
         <v>18.5</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H88" t="str">
-        <f>INT(E88/12) &amp; " ft " &amp; MOD(E88,12) &amp; " in"</f>
+      <c r="H89" s="3" t="str">
+        <f>INT(E89/12) &amp; " ft " &amp; MOD(E89,12) &amp; " in"</f>
         <v>2 ft 4.25 in</v>
       </c>
-      <c r="I88" s="2" t="s">
+      <c r="I89" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J88">
+      <c r="J89" s="3">
         <v>54</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="K89" s="3"/>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B89" t="s">
-        <v>51</v>
-      </c>
-      <c r="C89">
+      <c r="B90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C90" s="3">
         <v>2</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E89">
+      <c r="E90" s="3">
         <v>24.25</v>
       </c>
-      <c r="F89">
+      <c r="F90" s="3">
         <v>18.5</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G90" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H89" t="str">
-        <f>INT(E89/12) &amp; " ft " &amp; MOD(E89,12) &amp; " in"</f>
+      <c r="H90" s="3" t="str">
+        <f>INT(E90/12) &amp; " ft " &amp; MOD(E90,12) &amp; " in"</f>
         <v>2 ft 0.25 in</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I90" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J89">
+      <c r="J90" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B90" t="s">
-        <v>51</v>
-      </c>
-      <c r="C90">
+      <c r="B91" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C91" s="3">
         <v>2</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D91" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E90">
+      <c r="E91" s="3">
         <v>20.25</v>
       </c>
-      <c r="F90">
+      <c r="F91" s="3">
         <v>18.5</v>
       </c>
-      <c r="G90" t="s">
+      <c r="G91" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H90" t="str">
-        <f>INT(E90/12) &amp; " ft " &amp; MOD(E90,12) &amp; " in"</f>
+      <c r="H91" s="3" t="str">
+        <f>INT(E91/12) &amp; " ft " &amp; MOD(E91,12) &amp; " in"</f>
         <v>1 ft 8.25 in</v>
       </c>
-      <c r="I90" s="2" t="s">
+      <c r="I91" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J90">
+      <c r="J91" s="3">
         <v>56</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B91" t="s">
-        <v>51</v>
-      </c>
-      <c r="C91">
+      <c r="B92" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C92" s="3">
         <v>2</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D92" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E91">
+      <c r="E92" s="3">
         <v>16.25</v>
       </c>
-      <c r="F91">
+      <c r="F92" s="3">
         <v>18.5</v>
       </c>
-      <c r="G91" t="s">
+      <c r="G92" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H91" t="str">
-        <f>INT(E91/12) &amp; " ft " &amp; MOD(E91,12) &amp; " in"</f>
+      <c r="H92" s="3" t="str">
+        <f>INT(E92/12) &amp; " ft " &amp; MOD(E92,12) &amp; " in"</f>
         <v>1 ft 4.25 in</v>
       </c>
-      <c r="I91" s="2" t="s">
+      <c r="I92" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J91">
+      <c r="J92" s="3">
         <v>57</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+      <c r="M92" s="3"/>
+      <c r="N92" s="3"/>
+      <c r="O92" s="3"/>
+      <c r="P92" s="3"/>
+      <c r="Q92" s="3"/>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B92" t="s">
-        <v>51</v>
-      </c>
-      <c r="C92">
+      <c r="B93" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C93" s="3">
         <v>2</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E92">
+      <c r="E93" s="3">
         <v>12.25</v>
       </c>
-      <c r="F92">
+      <c r="F93" s="3">
         <v>18.5</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H92" t="str">
-        <f>INT(E92/12) &amp; " ft " &amp; MOD(E92,12) &amp; " in"</f>
+      <c r="H93" s="3" t="str">
+        <f>INT(E93/12) &amp; " ft " &amp; MOD(E93,12) &amp; " in"</f>
         <v>1 ft 0.25 in</v>
       </c>
-      <c r="I92" s="2" t="s">
+      <c r="I93" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J92">
+      <c r="J93" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="K93" s="3"/>
+      <c r="L93" s="3"/>
+      <c r="M93" s="3"/>
+      <c r="N93" s="3"/>
+      <c r="O93" s="3"/>
+      <c r="P93" s="3"/>
+      <c r="Q93" s="3"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B93" t="s">
-        <v>51</v>
-      </c>
-      <c r="C93">
+      <c r="B94" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C94" s="3">
         <v>2</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E93">
+      <c r="E94" s="3">
         <v>8.25</v>
       </c>
-      <c r="F93">
+      <c r="F94" s="3">
         <v>18.5</v>
       </c>
-      <c r="G93" t="s">
+      <c r="G94" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="H93" t="str">
-        <f>INT(E93/12) &amp; " ft " &amp; MOD(E93,12) &amp; " in"</f>
+      <c r="H94" s="3" t="str">
+        <f>INT(E94/12) &amp; " ft " &amp; MOD(E94,12) &amp; " in"</f>
         <v>0 ft 8.25 in</v>
       </c>
-      <c r="I93" s="2" t="s">
+      <c r="I94" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J93">
+      <c r="J94" s="3">
         <v>59</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+      <c r="M94" s="3"/>
+      <c r="N94" s="3"/>
+      <c r="O94" s="3"/>
+      <c r="P94" s="3"/>
+      <c r="Q94" s="3"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B94" t="s">
-        <v>51</v>
-      </c>
-      <c r="C94">
+      <c r="B95" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C95" s="3">
         <v>2</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D95" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E94">
+      <c r="E95" s="3">
         <v>144</v>
       </c>
-      <c r="F94">
-        <v>90</v>
-      </c>
-      <c r="H94" t="str">
-        <f>INT(E94/12) &amp; " ft " &amp; MOD(E94,12) &amp; " in"</f>
+      <c r="F95" s="3">
+        <v>90</v>
+      </c>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3" t="str">
+        <f>INT(E95/12) &amp; " ft " &amp; MOD(E95,12) &amp; " in"</f>
         <v>12 ft 0 in</v>
       </c>
-      <c r="I94" s="2" t="s">
+      <c r="I95" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J94">
+      <c r="J95" s="3">
         <v>118</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+      <c r="M95" s="3"/>
+      <c r="N95" s="3"/>
+      <c r="O95" s="3"/>
+      <c r="P95" s="3"/>
+      <c r="Q95" s="3"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>57</v>
-      </c>
-      <c r="B95" t="s">
-        <v>51</v>
-      </c>
-      <c r="C95">
-        <v>2</v>
-      </c>
-      <c r="D95" t="s">
-        <v>58</v>
-      </c>
-      <c r="E95">
-        <v>93</v>
-      </c>
-      <c r="F95">
-        <v>90</v>
-      </c>
-      <c r="H95" t="str">
-        <f>INT(E95/12) &amp; " ft " &amp; MOD(E95,12) &amp; " in"</f>
-        <v>7 ft 9 in</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J95">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>72</v>
       </c>
       <c r="B96" t="s">
         <v>51</v>
@@ -5268,28 +5553,25 @@
         <v>58</v>
       </c>
       <c r="E96">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="F96">
-        <v>18.5</v>
-      </c>
-      <c r="G96" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H96" t="str">
         <f>INT(E96/12) &amp; " ft " &amp; MOD(E96,12) &amp; " in"</f>
-        <v>2 ft 3 in</v>
+        <v>7 ft 9 in</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>79</v>
       </c>
       <c r="J96">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B97" t="s">
         <v>51</v>
@@ -5301,7 +5583,7 @@
         <v>58</v>
       </c>
       <c r="E97">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F97">
         <v>18.5</v>
@@ -5311,735 +5593,920 @@
       </c>
       <c r="H97" t="str">
         <f>INT(E97/12) &amp; " ft " &amp; MOD(E97,12) &amp; " in"</f>
-        <v>2 ft 6 in</v>
+        <v>2 ft 3 in</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>79</v>
       </c>
       <c r="J97">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B98" t="s">
         <v>51</v>
       </c>
       <c r="C98">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E98">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="F98">
-        <v>90</v>
+        <v>18.5</v>
+      </c>
+      <c r="G98" t="s">
+        <v>60</v>
       </c>
       <c r="H98" t="str">
         <f>INT(E98/12) &amp; " ft " &amp; MOD(E98,12) &amp; " in"</f>
-        <v>7 ft 4 in</v>
+        <v>2 ft 6 in</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>79</v>
       </c>
       <c r="J98">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C99" s="3">
+        <v>68</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E99" s="3">
+        <v>88</v>
+      </c>
+      <c r="F99" s="3">
+        <v>90</v>
+      </c>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3" t="str">
+        <f>INT(E99/12) &amp; " ft " &amp; MOD(E99,12) &amp; " in"</f>
+        <v>7 ft 4 in</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J99" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3"/>
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3"/>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B99" t="s">
-        <v>51</v>
-      </c>
-      <c r="C99">
+      <c r="B100" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C100" s="3">
         <v>8</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D100" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E99">
+      <c r="E100" s="3">
         <v>48</v>
       </c>
-      <c r="F99">
-        <v>90</v>
-      </c>
-      <c r="H99" t="str">
-        <f>INT(E99/12) &amp; " ft " &amp; MOD(E99,12) &amp; " in"</f>
+      <c r="F100" s="3">
+        <v>90</v>
+      </c>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3" t="str">
+        <f>INT(E100/12) &amp; " ft " &amp; MOD(E100,12) &amp; " in"</f>
         <v>4 ft 0 in</v>
       </c>
-      <c r="I99" s="2" t="s">
+      <c r="I100" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J99">
+      <c r="J100" s="3">
         <v>61</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="3"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="3"/>
+      <c r="P100" s="3"/>
+      <c r="Q100" s="3"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B100" t="s">
-        <v>51</v>
-      </c>
-      <c r="C100">
+      <c r="B101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C101" s="3">
         <v>8</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D101" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E100">
+      <c r="E101" s="3">
         <v>12</v>
       </c>
-      <c r="F100">
-        <v>90</v>
-      </c>
-      <c r="H100" t="str">
-        <f>INT(E100/12) &amp; " ft " &amp; MOD(E100,12) &amp; " in"</f>
+      <c r="F101" s="3">
+        <v>90</v>
+      </c>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3" t="str">
+        <f>INT(E101/12) &amp; " ft " &amp; MOD(E101,12) &amp; " in"</f>
         <v>1 ft 0 in</v>
       </c>
-      <c r="I100" s="2" t="s">
+      <c r="I101" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J100">
+      <c r="J101" s="3">
         <v>62</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="K101" s="3"/>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+      <c r="P101" s="3"/>
+      <c r="Q101" s="3"/>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B101" t="s">
-        <v>51</v>
-      </c>
-      <c r="C101">
+      <c r="B102" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C102" s="3">
         <v>2</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D102" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E101">
+      <c r="E102" s="3">
         <v>93</v>
       </c>
-      <c r="F101">
+      <c r="F102" s="3">
         <v>18.5</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H101" t="str">
-        <f>INT(E101/12) &amp; " ft " &amp; MOD(E101,12) &amp; " in"</f>
+      <c r="H102" s="3" t="str">
+        <f>INT(E102/12) &amp; " ft " &amp; MOD(E102,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="I102" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J101">
+      <c r="J102" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+      <c r="P102" s="3"/>
+      <c r="Q102" s="3"/>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B102" t="s">
-        <v>51</v>
-      </c>
-      <c r="C102">
+      <c r="B103" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C103" s="3">
         <v>2</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D103" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E102">
+      <c r="E103" s="3">
         <v>97</v>
       </c>
-      <c r="F102">
+      <c r="F103" s="3">
         <v>18.5</v>
       </c>
-      <c r="G102" t="s">
+      <c r="G103" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H102" t="str">
-        <f>INT(E102/12) &amp; " ft " &amp; MOD(E102,12) &amp; " in"</f>
+      <c r="H103" s="3" t="str">
+        <f>INT(E103/12) &amp; " ft " &amp; MOD(E103,12) &amp; " in"</f>
         <v>8 ft 1 in</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="I103" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J102">
+      <c r="J103" s="3">
         <v>64</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3"/>
+      <c r="P103" s="3"/>
+      <c r="Q103" s="3"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B103" t="s">
-        <v>51</v>
-      </c>
-      <c r="C103">
+      <c r="B104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="3">
         <v>2</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E103">
+      <c r="E104" s="3">
         <v>101</v>
       </c>
-      <c r="F103">
+      <c r="F104" s="3">
         <v>18.5</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G104" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H103" t="str">
-        <f>INT(E103/12) &amp; " ft " &amp; MOD(E103,12) &amp; " in"</f>
+      <c r="H104" s="3" t="str">
+        <f>INT(E104/12) &amp; " ft " &amp; MOD(E104,12) &amp; " in"</f>
         <v>8 ft 5 in</v>
       </c>
-      <c r="I103" s="2" t="s">
+      <c r="I104" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J103">
+      <c r="J104" s="3">
         <v>65</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="3"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="3"/>
+      <c r="P104" s="3"/>
+      <c r="Q104" s="3"/>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B104" t="s">
-        <v>51</v>
-      </c>
-      <c r="C104">
+      <c r="B105" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C105" s="3">
         <v>2</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D105" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E104">
+      <c r="E105" s="3">
         <v>109</v>
       </c>
-      <c r="F104">
+      <c r="F105" s="3">
         <v>18.5</v>
       </c>
-      <c r="G104" t="s">
+      <c r="G105" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H104" t="str">
-        <f>INT(E104/12) &amp; " ft " &amp; MOD(E104,12) &amp; " in"</f>
+      <c r="H105" s="3" t="str">
+        <f>INT(E105/12) &amp; " ft " &amp; MOD(E105,12) &amp; " in"</f>
         <v>9 ft 1 in</v>
       </c>
-      <c r="I104" s="2" t="s">
+      <c r="I105" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J104">
+      <c r="J105" s="3">
         <v>67</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+      <c r="M105" s="3"/>
+      <c r="N105" s="3"/>
+      <c r="O105" s="3"/>
+      <c r="P105" s="3"/>
+      <c r="Q105" s="3"/>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B105" t="s">
-        <v>51</v>
-      </c>
-      <c r="C105">
+      <c r="B106" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C106" s="3">
         <v>1</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D106" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E105">
+      <c r="E106" s="3">
         <v>112</v>
       </c>
-      <c r="F105">
+      <c r="F106" s="3">
         <v>18.5</v>
       </c>
-      <c r="G105" t="s">
+      <c r="G106" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="H105" t="str">
-        <f>INT(E105/12) &amp; " ft " &amp; MOD(E105,12) &amp; " in"</f>
+      <c r="H106" s="3" t="str">
+        <f>INT(E106/12) &amp; " ft " &amp; MOD(E106,12) &amp; " in"</f>
         <v>9 ft 4 in</v>
       </c>
-      <c r="I105" s="2" t="s">
+      <c r="I106" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J105">
+      <c r="J106" s="3">
         <v>68</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+      <c r="M106" s="3"/>
+      <c r="N106" s="3"/>
+      <c r="O106" s="3"/>
+      <c r="P106" s="3"/>
+      <c r="Q106" s="3"/>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B106" t="s">
-        <v>51</v>
-      </c>
-      <c r="C106">
+      <c r="B107" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C107" s="3">
         <v>2</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D107" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E106">
+      <c r="E107" s="3">
         <v>85</v>
       </c>
-      <c r="F106">
+      <c r="F107" s="3">
         <v>18.5</v>
       </c>
-      <c r="G106" t="s">
+      <c r="G107" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H106" t="str">
-        <f>INT(E106/12) &amp; " ft " &amp; MOD(E106,12) &amp; " in"</f>
+      <c r="H107" s="3" t="str">
+        <f>INT(E107/12) &amp; " ft " &amp; MOD(E107,12) &amp; " in"</f>
         <v>7 ft 1 in</v>
       </c>
-      <c r="I106" s="2" t="s">
+      <c r="I107" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J106">
+      <c r="J107" s="3">
         <v>69</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="3"/>
+      <c r="N107" s="3"/>
+      <c r="O107" s="3"/>
+      <c r="P107" s="3"/>
+      <c r="Q107" s="3"/>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B107" t="s">
-        <v>51</v>
-      </c>
-      <c r="C107">
+      <c r="B108" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C108" s="3">
         <v>2</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D108" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E107">
+      <c r="E108" s="3">
         <v>89</v>
       </c>
-      <c r="F107">
+      <c r="F108" s="3">
         <v>18.5</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G108" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H107" t="str">
-        <f>INT(E107/12) &amp; " ft " &amp; MOD(E107,12) &amp; " in"</f>
+      <c r="H108" s="3" t="str">
+        <f>INT(E108/12) &amp; " ft " &amp; MOD(E108,12) &amp; " in"</f>
         <v>7 ft 5 in</v>
       </c>
-      <c r="I107" s="2" t="s">
+      <c r="I108" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J107">
+      <c r="J108" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+      <c r="O108" s="3"/>
+      <c r="P108" s="3"/>
+      <c r="Q108" s="3"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B108" t="s">
-        <v>51</v>
-      </c>
-      <c r="C108">
+      <c r="B109" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C109" s="3">
         <v>2</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D109" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E108">
+      <c r="E109" s="3">
         <v>93</v>
       </c>
-      <c r="F108">
+      <c r="F109" s="3">
         <v>18.5</v>
       </c>
-      <c r="G108" t="s">
+      <c r="G109" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H108" t="str">
-        <f>INT(E108/12) &amp; " ft " &amp; MOD(E108,12) &amp; " in"</f>
+      <c r="H109" s="3" t="str">
+        <f>INT(E109/12) &amp; " ft " &amp; MOD(E109,12) &amp; " in"</f>
         <v>7 ft 9 in</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="I109" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J108">
+      <c r="J109" s="3">
         <v>71</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+      <c r="M109" s="3"/>
+      <c r="N109" s="3"/>
+      <c r="O109" s="3"/>
+      <c r="P109" s="3"/>
+      <c r="Q109" s="3"/>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B109" t="s">
-        <v>51</v>
-      </c>
-      <c r="C109">
+      <c r="B110" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C110" s="3">
         <v>2</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D110" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E109">
+      <c r="E110" s="3">
         <v>97</v>
       </c>
-      <c r="F109">
+      <c r="F110" s="3">
         <v>18.5</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G110" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H109" t="str">
-        <f>INT(E109/12) &amp; " ft " &amp; MOD(E109,12) &amp; " in"</f>
+      <c r="H110" s="3" t="str">
+        <f>INT(E110/12) &amp; " ft " &amp; MOD(E110,12) &amp; " in"</f>
         <v>8 ft 1 in</v>
       </c>
-      <c r="I109" s="2" t="s">
+      <c r="I110" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J109">
+      <c r="J110" s="3">
         <v>72</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+      <c r="M110" s="3"/>
+      <c r="N110" s="3"/>
+      <c r="O110" s="3"/>
+      <c r="P110" s="3"/>
+      <c r="Q110" s="3"/>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B110" t="s">
-        <v>51</v>
-      </c>
-      <c r="C110">
+      <c r="B111" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C111" s="3">
         <v>2</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D111" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E110">
+      <c r="E111" s="3">
         <v>16</v>
       </c>
-      <c r="F110">
+      <c r="F111" s="3">
         <v>18.5</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G111" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H110" t="str">
-        <f>INT(E110/12) &amp; " ft " &amp; MOD(E110,12) &amp; " in"</f>
+      <c r="H111" s="3" t="str">
+        <f>INT(E111/12) &amp; " ft " &amp; MOD(E111,12) &amp; " in"</f>
         <v>1 ft 4 in</v>
       </c>
-      <c r="I110" s="2" t="s">
+      <c r="I111" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J110">
+      <c r="J111" s="3">
         <v>73</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="K111" s="3"/>
+      <c r="L111" s="3"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="3"/>
+      <c r="P111" s="3"/>
+      <c r="Q111" s="3"/>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B111" t="s">
-        <v>51</v>
-      </c>
-      <c r="C111">
+      <c r="B112" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C112" s="3">
         <v>2</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D112" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E111">
+      <c r="E112" s="3">
         <v>19</v>
       </c>
-      <c r="F111">
+      <c r="F112" s="3">
         <v>18.5</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G112" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H111" t="str">
-        <f>INT(E111/12) &amp; " ft " &amp; MOD(E111,12) &amp; " in"</f>
+      <c r="H112" s="3" t="str">
+        <f>INT(E112/12) &amp; " ft " &amp; MOD(E112,12) &amp; " in"</f>
         <v>1 ft 7 in</v>
       </c>
-      <c r="I111" s="2" t="s">
+      <c r="I112" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J111">
+      <c r="J112" s="3">
         <v>74</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
+      <c r="M112" s="3"/>
+      <c r="N112" s="3"/>
+      <c r="O112" s="3"/>
+      <c r="P112" s="3"/>
+      <c r="Q112" s="3"/>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B112" t="s">
-        <v>51</v>
-      </c>
-      <c r="C112">
+      <c r="B113" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C113" s="3">
         <v>1</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D113" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E112">
+      <c r="E113" s="3">
         <v>20</v>
       </c>
-      <c r="F112">
-        <v>90</v>
-      </c>
-      <c r="H112" t="str">
-        <f>INT(E112/12) &amp; " ft " &amp; MOD(E112,12) &amp; " in"</f>
+      <c r="F113" s="3">
+        <v>90</v>
+      </c>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3" t="str">
+        <f>INT(E113/12) &amp; " ft " &amp; MOD(E113,12) &amp; " in"</f>
         <v>1 ft 8 in</v>
       </c>
-      <c r="I112" s="2" t="s">
+      <c r="I113" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J112">
+      <c r="J113" s="3">
         <v>75</v>
       </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="K113" s="3"/>
+      <c r="L113" s="3"/>
+      <c r="M113" s="3"/>
+      <c r="N113" s="3"/>
+      <c r="O113" s="3"/>
+      <c r="P113" s="3"/>
+      <c r="Q113" s="3"/>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B113" t="s">
-        <v>51</v>
-      </c>
-      <c r="C113">
+      <c r="B114" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C114" s="3">
         <v>4</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E113">
+      <c r="E114" s="3">
         <v>6</v>
       </c>
-      <c r="F113">
+      <c r="F114" s="3">
         <v>18.5</v>
       </c>
-      <c r="G113" t="s">
+      <c r="G114" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H113" t="str">
-        <f>INT(E113/12) &amp; " ft " &amp; MOD(E113,12) &amp; " in"</f>
+      <c r="H114" s="3" t="str">
+        <f>INT(E114/12) &amp; " ft " &amp; MOD(E114,12) &amp; " in"</f>
         <v>0 ft 6 in</v>
       </c>
-      <c r="I113" s="2" t="s">
+      <c r="I114" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J113">
+      <c r="J114" s="3">
         <v>76</v>
       </c>
-    </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="K114" s="3"/>
+      <c r="L114" s="3"/>
+      <c r="M114" s="3"/>
+      <c r="N114" s="3"/>
+      <c r="O114" s="3"/>
+      <c r="P114" s="3"/>
+      <c r="Q114" s="3"/>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B114" t="s">
-        <v>51</v>
-      </c>
-      <c r="C114">
+      <c r="B115" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C115" s="3">
         <v>2</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D115" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E114">
+      <c r="E115" s="3">
         <v>10</v>
       </c>
-      <c r="F114">
+      <c r="F115" s="3">
         <v>18.5</v>
       </c>
-      <c r="G114" t="s">
+      <c r="G115" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H114" t="str">
-        <f>INT(E114/12) &amp; " ft " &amp; MOD(E114,12) &amp; " in"</f>
+      <c r="H115" s="3" t="str">
+        <f>INT(E115/12) &amp; " ft " &amp; MOD(E115,12) &amp; " in"</f>
         <v>0 ft 10 in</v>
       </c>
-      <c r="I114" s="2" t="s">
+      <c r="I115" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J114">
+      <c r="J115" s="3">
         <v>77</v>
       </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="K115" s="3"/>
+      <c r="L115" s="3"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="O115" s="3"/>
+      <c r="P115" s="3"/>
+      <c r="Q115" s="3"/>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B115" t="s">
-        <v>51</v>
-      </c>
-      <c r="C115">
+      <c r="B116" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C116" s="3">
         <v>2</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D116" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E115">
+      <c r="E116" s="3">
         <v>14</v>
       </c>
-      <c r="F115">
+      <c r="F116" s="3">
         <v>18.5</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G116" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H115" t="str">
-        <f>INT(E115/12) &amp; " ft " &amp; MOD(E115,12) &amp; " in"</f>
+      <c r="H116" s="3" t="str">
+        <f>INT(E116/12) &amp; " ft " &amp; MOD(E116,12) &amp; " in"</f>
         <v>1 ft 2 in</v>
       </c>
-      <c r="I115" s="2" t="s">
+      <c r="I116" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J115">
+      <c r="J116" s="3">
         <v>78</v>
       </c>
-    </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="3"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="3"/>
+      <c r="P116" s="3"/>
+      <c r="Q116" s="3"/>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B116" t="s">
-        <v>51</v>
-      </c>
-      <c r="C116">
+      <c r="B117" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C117" s="3">
         <v>2</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D117" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E116">
+      <c r="E117" s="3">
         <v>18</v>
       </c>
-      <c r="F116">
+      <c r="F117" s="3">
         <v>18.5</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G117" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H116" t="str">
-        <f>INT(E116/12) &amp; " ft " &amp; MOD(E116,12) &amp; " in"</f>
+      <c r="H117" s="3" t="str">
+        <f>INT(E117/12) &amp; " ft " &amp; MOD(E117,12) &amp; " in"</f>
         <v>1 ft 6 in</v>
       </c>
-      <c r="I116" s="2" t="s">
+      <c r="I117" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J116">
+      <c r="J117" s="3">
         <v>79</v>
       </c>
-    </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="K117" s="3"/>
+      <c r="L117" s="3"/>
+      <c r="M117" s="3"/>
+      <c r="N117" s="3"/>
+      <c r="O117" s="3"/>
+      <c r="P117" s="3"/>
+      <c r="Q117" s="3"/>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B117" t="s">
-        <v>51</v>
-      </c>
-      <c r="C117">
+      <c r="B118" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C118" s="3">
         <v>1</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D118" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E117">
+      <c r="E118" s="3">
         <v>22</v>
       </c>
-      <c r="F117">
+      <c r="F118" s="3">
         <v>18.5</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G118" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H117" t="str">
-        <f>INT(E117/12) &amp; " ft " &amp; MOD(E117,12) &amp; " in"</f>
+      <c r="H118" s="3" t="str">
+        <f>INT(E118/12) &amp; " ft " &amp; MOD(E118,12) &amp; " in"</f>
         <v>1 ft 10 in</v>
       </c>
-      <c r="I117" s="2" t="s">
+      <c r="I118" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J117">
+      <c r="J118" s="3">
         <v>80</v>
       </c>
-    </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="3"/>
+      <c r="P118" s="3"/>
+      <c r="Q118" s="3"/>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B118" t="s">
-        <v>51</v>
-      </c>
-      <c r="C118">
+      <c r="B119" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C119" s="3">
         <v>10</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D119" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E118">
+      <c r="E119" s="3">
         <v>120</v>
       </c>
-      <c r="F118">
-        <v>90</v>
-      </c>
-      <c r="H118" t="str">
-        <f>INT(E118/12) &amp; " ft " &amp; MOD(E118,12) &amp; " in"</f>
+      <c r="F119" s="3">
+        <v>90</v>
+      </c>
+      <c r="G119" s="3"/>
+      <c r="H119" s="3" t="str">
+        <f>INT(E119/12) &amp; " ft " &amp; MOD(E119,12) &amp; " in"</f>
         <v>10 ft 0 in</v>
       </c>
-      <c r="I118" s="2" t="s">
+      <c r="I119" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="J118">
+      <c r="J119" s="3">
         <v>81</v>
       </c>
-    </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>90</v>
-      </c>
-      <c r="B119" t="s">
-        <v>51</v>
-      </c>
-      <c r="C119">
+      <c r="K119" s="3"/>
+      <c r="L119" s="3"/>
+      <c r="M119" s="3"/>
+      <c r="N119" s="3"/>
+      <c r="O119" s="3"/>
+      <c r="P119" s="3"/>
+      <c r="Q119" s="3"/>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>90</v>
+      </c>
+      <c r="B120" t="s">
+        <v>51</v>
+      </c>
+      <c r="C120">
         <v>2</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D120" t="s">
         <v>91</v>
       </c>
-      <c r="E119">
+      <c r="E120">
         <v>105</v>
       </c>
-      <c r="F119">
+      <c r="F120">
         <v>18.5</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G120" t="s">
         <v>60</v>
       </c>
-      <c r="H119" t="str">
-        <f>INT(E119/12) &amp; " ft " &amp; MOD(E119,12) &amp; " in"</f>
+      <c r="H120" t="str">
+        <f>INT(E120/12) &amp; " ft " &amp; MOD(E120,12) &amp; " in"</f>
         <v>8 ft 9 in</v>
       </c>
-      <c r="I119" s="2" t="s">
+      <c r="I120" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J119">
+      <c r="J120">
         <v>66</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P120">
-        <f>SUM(P2:P119)</f>
-        <v>2243.8699999999994</v>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P121">
+        <f>SUM(P2:P120)</f>
+        <v>2373.5699999999993</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J119">
-    <sortCondition descending="1" ref="D2:D119"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J120">
+    <sortCondition descending="1" ref="D2:D120"/>
   </sortState>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Added 1x12 board prices
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F01C4DCA-BBEE-9B4F-9241-7D6B1ED76A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8B1543A9-6C79-6C4A-BF93-5655955C1AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="-21100" windowWidth="27420" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
+    <workbookView xWindow="6340" yWindow="-21100" windowWidth="26600" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="594" uniqueCount="189">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="598" uniqueCount="189">
   <si>
     <t>FLOOR</t>
   </si>
@@ -1492,8 +1492,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0679CAE-7790-0146-A436-E7EEAE9C9294}">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="Q55" sqref="Q55"/>
+    <sheetView tabSelected="1" topLeftCell="G51" workbookViewId="0">
+      <selection activeCell="R76" sqref="R76:R79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4379,7 +4379,7 @@
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>134</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>141</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>143</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>147</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>148</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>149</v>
       </c>
@@ -4609,7 +4609,7 @@
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>151</v>
       </c>
@@ -4647,7 +4647,7 @@
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>152</v>
       </c>
@@ -4687,7 +4687,7 @@
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>50</v>
       </c>
@@ -4778,14 +4778,29 @@
         <v>35</v>
       </c>
       <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="3"/>
-      <c r="O76" s="3"/>
-      <c r="P76" s="3"/>
+      <c r="L76" s="3">
+        <v>96</v>
+      </c>
+      <c r="M76" s="3" t="str">
+        <f t="shared" ref="M76:M79" si="9">INT(L76/12) &amp; " ft "</f>
+        <v xml:space="preserve">8 ft </v>
+      </c>
+      <c r="N76" s="3">
+        <v>65</v>
+      </c>
+      <c r="O76" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="P76" s="3">
+        <f>O76*N76</f>
+        <v>468</v>
+      </c>
       <c r="Q76" s="3"/>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R76" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>53</v>
       </c>
@@ -4816,14 +4831,29 @@
         <v>36</v>
       </c>
       <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
+      <c r="L77" s="3">
+        <v>120</v>
+      </c>
+      <c r="M77" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">10 ft </v>
+      </c>
+      <c r="N77" s="3">
+        <v>18</v>
+      </c>
+      <c r="O77" s="3">
+        <v>9</v>
+      </c>
+      <c r="P77" s="3">
+        <f t="shared" ref="P77:P79" si="10">O77*N77</f>
+        <v>162</v>
+      </c>
       <c r="Q77" s="3"/>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R77" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>54</v>
       </c>
@@ -4854,14 +4884,29 @@
         <v>37</v>
       </c>
       <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
+      <c r="L78" s="3">
+        <v>144</v>
+      </c>
+      <c r="M78" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">12 ft </v>
+      </c>
+      <c r="N78" s="3">
+        <v>3</v>
+      </c>
+      <c r="O78" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="P78" s="3">
+        <f t="shared" si="10"/>
+        <v>34.200000000000003</v>
+      </c>
       <c r="Q78" s="3"/>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>59</v>
       </c>
@@ -4894,14 +4939,29 @@
         <v>41</v>
       </c>
       <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3"/>
-      <c r="O79" s="3"/>
-      <c r="P79" s="3"/>
+      <c r="L79" s="3">
+        <v>168</v>
+      </c>
+      <c r="M79" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">14 ft </v>
+      </c>
+      <c r="N79" s="3">
+        <v>3</v>
+      </c>
+      <c r="O79" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="P79" s="3">
+        <f t="shared" si="10"/>
+        <v>39.900000000000006</v>
+      </c>
       <c r="Q79" s="3"/>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R79" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>61</v>
       </c>
@@ -5537,7 +5597,10 @@
       <c r="N95" s="3"/>
       <c r="O95" s="3"/>
       <c r="P95" s="3"/>
-      <c r="Q95" s="3"/>
+      <c r="Q95" s="3">
+        <f>SUM(P76:P79)</f>
+        <v>704.1</v>
+      </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -6501,7 +6564,7 @@
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P121">
         <f>SUM(P2:P120)</f>
-        <v>2373.5699999999993</v>
+        <v>3077.6699999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 1x5 board prices
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/IdeaProjects/cabin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F7C1D34F-E638-B941-8DC5-0C6B26758AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{427DCE16-FDDF-8844-ACC3-45F3EA0C486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="-21100" windowWidth="28000" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
+    <workbookView xWindow="4360" yWindow="-21100" windowWidth="28940" windowHeight="20300" xr2:uid="{E053DE24-4FBD-1846-80E5-1FECEB30610C}"/>
   </bookViews>
   <sheets>
     <sheet name="floor_2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="601" uniqueCount="189">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="604" uniqueCount="192">
   <si>
     <t>FLOOR</t>
   </si>
@@ -603,6 +603,15 @@
   </si>
   <si>
     <t>https://www.hepsales.com/cdx-plywood-3-4-in-x-4-ft-x-8-ft-pine/</t>
+  </si>
+  <si>
+    <t>Lumber Total</t>
+  </si>
+  <si>
+    <t>didn't have 1x5 at sawmill so used 1x6 prices</t>
+  </si>
+  <si>
+    <t>would need to have custom cut or find different supplier</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1501,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0679CAE-7790-0146-A436-E7EEAE9C9294}">
   <dimension ref="A1:R121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G72" workbookViewId="0">
-      <selection activeCell="R99" sqref="R99:R101"/>
+    <sheetView tabSelected="1" topLeftCell="G35" workbookViewId="0">
+      <selection activeCell="R58" sqref="R58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4045,6 +4054,26 @@
       <c r="J55">
         <v>96</v>
       </c>
+      <c r="L55" s="2">
+        <v>96</v>
+      </c>
+      <c r="M55" s="2" t="str">
+        <f t="shared" ref="M55:M57" si="9">INT(L55/12) &amp; " ft "</f>
+        <v xml:space="preserve">8 ft </v>
+      </c>
+      <c r="N55" s="2">
+        <v>1</v>
+      </c>
+      <c r="O55" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="P55">
+        <f>O55*N55</f>
+        <v>3.6</v>
+      </c>
+      <c r="R55" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
@@ -4078,6 +4107,26 @@
       <c r="J56">
         <v>98</v>
       </c>
+      <c r="L56" s="2">
+        <v>120</v>
+      </c>
+      <c r="M56" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">10 ft </v>
+      </c>
+      <c r="N56" s="2">
+        <v>1</v>
+      </c>
+      <c r="O56" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="P56">
+        <f t="shared" ref="P56:P57" si="10">O56*N56</f>
+        <v>4.5</v>
+      </c>
+      <c r="R56" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -4107,6 +4156,27 @@
       </c>
       <c r="J57">
         <v>99</v>
+      </c>
+      <c r="L57" s="2">
+        <v>168</v>
+      </c>
+      <c r="M57" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">14 ft </v>
+      </c>
+      <c r="N57" s="2">
+        <v>1</v>
+      </c>
+      <c r="O57" s="2">
+        <v>6.65</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="10"/>
+        <v>6.65</v>
+      </c>
+      <c r="Q57">
+        <f>SUM(P55:P57)</f>
+        <v>14.75</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
@@ -4782,7 +4852,7 @@
         <v>96</v>
       </c>
       <c r="M76" s="3" t="str">
-        <f t="shared" ref="M76:M79" si="9">INT(L76/12) &amp; " ft "</f>
+        <f t="shared" ref="M76:M79" si="11">INT(L76/12) &amp; " ft "</f>
         <v xml:space="preserve">8 ft </v>
       </c>
       <c r="N76" s="3">
@@ -4835,7 +4905,7 @@
         <v>120</v>
       </c>
       <c r="M77" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">10 ft </v>
       </c>
       <c r="N77" s="3">
@@ -4845,7 +4915,7 @@
         <v>9</v>
       </c>
       <c r="P77" s="3">
-        <f t="shared" ref="P77:P79" si="10">O77*N77</f>
+        <f t="shared" ref="P77:P79" si="12">O77*N77</f>
         <v>162</v>
       </c>
       <c r="Q77" s="3"/>
@@ -4888,7 +4958,7 @@
         <v>144</v>
       </c>
       <c r="M78" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">12 ft </v>
       </c>
       <c r="N78" s="3">
@@ -4898,7 +4968,7 @@
         <v>11.4</v>
       </c>
       <c r="P78" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>34.200000000000003</v>
       </c>
       <c r="Q78" s="3"/>
@@ -4943,7 +5013,7 @@
         <v>168</v>
       </c>
       <c r="M79" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">14 ft </v>
       </c>
       <c r="N79" s="3">
@@ -4953,7 +5023,7 @@
         <v>13.3</v>
       </c>
       <c r="P79" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>39.900000000000006</v>
       </c>
       <c r="Q79" s="3"/>
@@ -5733,7 +5803,7 @@
         <v>96</v>
       </c>
       <c r="M99" s="3" t="str">
-        <f t="shared" ref="M99:M101" si="11">INT(L99/12) &amp; " ft "</f>
+        <f t="shared" ref="M99:M101" si="13">INT(L99/12) &amp; " ft "</f>
         <v xml:space="preserve">8 ft </v>
       </c>
       <c r="N99" s="3">
@@ -5786,7 +5856,7 @@
         <v>120</v>
       </c>
       <c r="M100" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">10 ft </v>
       </c>
       <c r="N100" s="3">
@@ -5796,7 +5866,7 @@
         <v>2.25</v>
       </c>
       <c r="P100" s="3">
-        <f t="shared" ref="P100:P101" si="12">O100*N100</f>
+        <f t="shared" ref="P100:P101" si="14">O100*N100</f>
         <v>38.25</v>
       </c>
       <c r="Q100" s="3"/>
@@ -5839,7 +5909,7 @@
         <v>192</v>
       </c>
       <c r="M101" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v xml:space="preserve">16 ft </v>
       </c>
       <c r="N101" s="3">
@@ -5849,7 +5919,7 @@
         <v>3.8</v>
       </c>
       <c r="P101" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>60.8</v>
       </c>
       <c r="Q101" s="3"/>
@@ -6297,7 +6367,7 @@
       <c r="P112" s="3"/>
       <c r="Q112" s="3"/>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>101</v>
       </c>
@@ -6335,7 +6405,7 @@
       <c r="P113" s="3"/>
       <c r="Q113" s="3"/>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>102</v>
       </c>
@@ -6375,7 +6445,7 @@
       <c r="P114" s="3"/>
       <c r="Q114" s="3"/>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>104</v>
       </c>
@@ -6415,7 +6485,7 @@
       <c r="P115" s="3"/>
       <c r="Q115" s="3"/>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>105</v>
       </c>
@@ -6455,7 +6525,7 @@
       <c r="P116" s="3"/>
       <c r="Q116" s="3"/>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>106</v>
       </c>
@@ -6495,7 +6565,7 @@
       <c r="P117" s="3"/>
       <c r="Q117" s="3"/>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>107</v>
       </c>
@@ -6535,7 +6605,7 @@
       <c r="P118" s="3"/>
       <c r="Q118" s="3"/>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>109</v>
       </c>
@@ -6576,7 +6646,7 @@
         <v>189.05</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>90</v>
       </c>
@@ -6609,10 +6679,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="P121">
         <f>SUM(P2:P120)</f>
-        <v>3266.7199999999993</v>
+        <v>3281.4699999999993</v>
+      </c>
+      <c r="R121" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>